<commit_message>
National accounts - Volume
</commit_message>
<xml_diff>
--- a/output1.xlsx
+++ b/output1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="197">
   <si>
     <t>Country Ameco</t>
   </si>
@@ -962,7 +962,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE195"/>
+  <dimension ref="A1:AE189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -13094,7 +13094,7 @@
         <v>4</v>
       </c>
       <c r="B144" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C144" t="s">
         <v>193</v>
@@ -13102,35 +13102,23 @@
       <c r="D144" t="s">
         <v>194</v>
       </c>
-      <c r="V144">
-        <v>-0.055</v>
-      </c>
-      <c r="W144">
-        <v>-0.406</v>
-      </c>
-      <c r="X144">
-        <v>1.4992</v>
-      </c>
-      <c r="Y144">
-        <v>2.498</v>
-      </c>
       <c r="Z144">
-        <v>1.86</v>
+        <v>-0.4109</v>
       </c>
       <c r="AA144">
-        <v>0.64</v>
+        <v>-0.1896</v>
       </c>
       <c r="AB144">
-        <v>0.7979999999999999</v>
+        <v>-0.08</v>
       </c>
       <c r="AC144">
-        <v>2.002</v>
+        <v>-0.063</v>
       </c>
       <c r="AD144">
-        <v>1.71325</v>
+        <v>-0.062</v>
       </c>
       <c r="AE144">
-        <v>1.5015</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="145" spans="1:31">
@@ -13138,7 +13126,7 @@
         <v>4</v>
       </c>
       <c r="B145" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C145" t="s">
         <v>193</v>
@@ -13146,6 +13134,18 @@
       <c r="D145" t="s">
         <v>194</v>
       </c>
+      <c r="V145">
+        <v>0.145</v>
+      </c>
+      <c r="W145">
+        <v>-0.358</v>
+      </c>
+      <c r="X145">
+        <v>-2.9</v>
+      </c>
+      <c r="Y145">
+        <v>0.009000000000000001</v>
+      </c>
       <c r="Z145">
         <v>-0.4109</v>
       </c>
@@ -13170,7 +13170,7 @@
         <v>4</v>
       </c>
       <c r="B146" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C146" t="s">
         <v>193</v>
@@ -13178,35 +13178,68 @@
       <c r="D146" t="s">
         <v>194</v>
       </c>
+      <c r="H146">
+        <v>-0.1088971269694161</v>
+      </c>
+      <c r="I146">
+        <v>-0.2160565338276182</v>
+      </c>
+      <c r="J146">
+        <v>-0.2930954587581094</v>
+      </c>
+      <c r="K146">
+        <v>-0.2939643188137164</v>
+      </c>
+      <c r="L146">
+        <v>-0.2314063948100093</v>
+      </c>
+      <c r="M146">
+        <v>-0.1859360518999074</v>
+      </c>
+      <c r="N146">
+        <v>-0.147126969416126</v>
+      </c>
+      <c r="O146">
+        <v>-0.406047265987025</v>
+      </c>
+      <c r="P146">
+        <v>-0.3527571825764598</v>
+      </c>
+      <c r="T146">
+        <v>-1.169</v>
+      </c>
+      <c r="U146">
+        <v>0.454</v>
+      </c>
       <c r="V146">
-        <v>0.145</v>
+        <v>-0.598</v>
       </c>
       <c r="W146">
-        <v>-0.358</v>
+        <v>-1.215</v>
       </c>
       <c r="X146">
-        <v>-2.9</v>
+        <v>-1.047</v>
       </c>
       <c r="Y146">
-        <v>0.009000000000000001</v>
+        <v>-0.955</v>
       </c>
       <c r="Z146">
-        <v>-0.4109</v>
+        <v>-0.507</v>
       </c>
       <c r="AA146">
-        <v>-0.1896</v>
+        <v>-1.554</v>
       </c>
       <c r="AB146">
-        <v>-0.08</v>
+        <v>-1.543</v>
       </c>
       <c r="AC146">
-        <v>-0.063</v>
+        <v>-1.51657</v>
       </c>
       <c r="AD146">
-        <v>-0.062</v>
+        <v>-1.546837625</v>
       </c>
       <c r="AE146">
-        <v>-0.04</v>
+        <v>-1.577743952125</v>
       </c>
     </row>
     <row r="147" spans="1:31">
@@ -13214,7 +13247,7 @@
         <v>4</v>
       </c>
       <c r="B147" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C147" t="s">
         <v>193</v>
@@ -13222,35 +13255,86 @@
       <c r="D147" t="s">
         <v>194</v>
       </c>
+      <c r="E147">
+        <v>2.833</v>
+      </c>
+      <c r="F147">
+        <v>4.519</v>
+      </c>
+      <c r="G147">
+        <v>4.5268</v>
+      </c>
+      <c r="H147">
+        <v>4.8832</v>
+      </c>
+      <c r="I147">
+        <v>5.3498</v>
+      </c>
+      <c r="J147">
+        <v>5.5431</v>
+      </c>
+      <c r="K147">
+        <v>5.5335</v>
+      </c>
+      <c r="L147">
+        <v>6.4918</v>
+      </c>
+      <c r="M147">
+        <v>4.8235</v>
+      </c>
+      <c r="N147">
+        <v>4.5738</v>
+      </c>
+      <c r="O147">
+        <v>5.212999999999999</v>
+      </c>
+      <c r="P147">
+        <v>3.9553</v>
+      </c>
+      <c r="Q147">
+        <v>3.6537</v>
+      </c>
+      <c r="R147">
+        <v>4.4317</v>
+      </c>
+      <c r="S147">
+        <v>4.5229</v>
+      </c>
+      <c r="T147">
+        <v>8.300599999999999</v>
+      </c>
+      <c r="U147">
+        <v>0.4297</v>
+      </c>
       <c r="V147">
-        <v>0.145</v>
+        <v>11.5077</v>
       </c>
       <c r="W147">
-        <v>-0.358</v>
+        <v>3.8228</v>
       </c>
       <c r="X147">
-        <v>-2.9</v>
+        <v>9.4825</v>
       </c>
       <c r="Y147">
-        <v>0.009000000000000001</v>
+        <v>6.4686</v>
       </c>
       <c r="Z147">
-        <v>-0.511</v>
+        <v>2.7633</v>
       </c>
       <c r="AA147">
-        <v>-0.21</v>
+        <v>-1.165</v>
       </c>
       <c r="AB147">
-        <v>-0.9732</v>
+        <v>2.5929</v>
       </c>
       <c r="AC147">
-        <v>-0.196</v>
+        <v>0.1555</v>
       </c>
       <c r="AD147">
-        <v>-0.1928888888888889</v>
+        <v>-1.546837625</v>
       </c>
       <c r="AE147">
-        <v>-0.1244444444444444</v>
+        <v>-1.577743952125</v>
       </c>
     </row>
     <row r="148" spans="1:31">
@@ -13258,7 +13342,7 @@
         <v>4</v>
       </c>
       <c r="B148" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C148" t="s">
         <v>193</v>
@@ -13266,68 +13350,41 @@
       <c r="D148" t="s">
         <v>194</v>
       </c>
-      <c r="H148">
-        <v>-0.1088971269694161</v>
-      </c>
-      <c r="I148">
-        <v>-0.2160565338276182</v>
-      </c>
-      <c r="J148">
-        <v>-0.2930954587581094</v>
-      </c>
-      <c r="K148">
-        <v>-0.2939643188137164</v>
-      </c>
-      <c r="L148">
-        <v>-0.2314063948100093</v>
-      </c>
-      <c r="M148">
-        <v>-0.1859360518999074</v>
-      </c>
-      <c r="N148">
-        <v>-0.147126969416126</v>
-      </c>
-      <c r="O148">
-        <v>-0.406047265987025</v>
-      </c>
-      <c r="P148">
-        <v>-0.3527571825764598</v>
-      </c>
       <c r="T148">
-        <v>-1.169</v>
+        <v>0.595</v>
       </c>
       <c r="U148">
-        <v>0.454</v>
+        <v>0.521</v>
       </c>
       <c r="V148">
-        <v>-0.598</v>
+        <v>0.959</v>
       </c>
       <c r="W148">
-        <v>-1.215</v>
+        <v>0.748</v>
       </c>
       <c r="X148">
-        <v>-1.047</v>
+        <v>0.404</v>
       </c>
       <c r="Y148">
-        <v>-0.955</v>
+        <v>0.972</v>
       </c>
       <c r="Z148">
-        <v>-0.507</v>
+        <v>1.169</v>
       </c>
       <c r="AA148">
-        <v>-1.554</v>
+        <v>0.9460000000000001</v>
       </c>
       <c r="AB148">
-        <v>-1.543</v>
+        <v>0.7880799999999998</v>
       </c>
       <c r="AC148">
-        <v>-1.51657</v>
+        <v>0.8164984079999998</v>
       </c>
       <c r="AD148">
-        <v>-1.546837625</v>
+        <v>0.8534050686799997</v>
       </c>
       <c r="AE148">
-        <v>-1.577743952125</v>
+        <v>0.8881932261977996</v>
       </c>
     </row>
     <row r="149" spans="1:31">
@@ -13335,7 +13392,7 @@
         <v>4</v>
       </c>
       <c r="B149" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C149" t="s">
         <v>193</v>
@@ -13344,85 +13401,85 @@
         <v>194</v>
       </c>
       <c r="E149">
-        <v>2.833</v>
+        <v>-1.27</v>
       </c>
       <c r="F149">
-        <v>4.519</v>
+        <v>-1.524</v>
       </c>
       <c r="G149">
-        <v>4.5268</v>
+        <v>-2.2978</v>
       </c>
       <c r="H149">
-        <v>4.8832</v>
+        <v>-2.8219</v>
       </c>
       <c r="I149">
-        <v>5.3498</v>
+        <v>-2.773</v>
       </c>
       <c r="J149">
-        <v>5.5431</v>
+        <v>-3.0305</v>
       </c>
       <c r="K149">
-        <v>5.5335</v>
+        <v>-3.075</v>
       </c>
       <c r="L149">
-        <v>6.4918</v>
+        <v>-3.0748</v>
       </c>
       <c r="M149">
-        <v>4.8235</v>
+        <v>-2.7424</v>
       </c>
       <c r="N149">
-        <v>4.5738</v>
+        <v>-3.198</v>
       </c>
       <c r="O149">
-        <v>5.212999999999999</v>
+        <v>-3.9897</v>
       </c>
       <c r="P149">
-        <v>3.9553</v>
+        <v>-4.4644</v>
       </c>
       <c r="Q149">
-        <v>3.6537</v>
+        <v>-4.5106</v>
       </c>
       <c r="R149">
-        <v>4.4317</v>
+        <v>-4.59</v>
       </c>
       <c r="S149">
-        <v>4.5229</v>
+        <v>-3.9447</v>
       </c>
       <c r="T149">
-        <v>8.300599999999999</v>
+        <v>-5.2088</v>
       </c>
       <c r="U149">
-        <v>0.4297</v>
+        <v>-5.3024</v>
       </c>
       <c r="V149">
-        <v>11.5077</v>
+        <v>-4.5547</v>
       </c>
       <c r="W149">
-        <v>3.8228</v>
+        <v>-4.9039</v>
       </c>
       <c r="X149">
-        <v>9.4825</v>
+        <v>-6.0074</v>
       </c>
       <c r="Y149">
-        <v>6.4686</v>
+        <v>-6.7782</v>
       </c>
       <c r="Z149">
-        <v>2.7633</v>
+        <v>-6.4232</v>
       </c>
       <c r="AA149">
-        <v>-1.165</v>
+        <v>-6.4025</v>
       </c>
       <c r="AB149">
-        <v>2.5929</v>
+        <v>-7.9044</v>
       </c>
       <c r="AC149">
-        <v>0.1555</v>
+        <v>-6.7732</v>
       </c>
       <c r="AD149">
-        <v>-1.546837625</v>
+        <v>0.8534050686799997</v>
       </c>
       <c r="AE149">
-        <v>-1.577743952125</v>
+        <v>0.8881932261977996</v>
       </c>
     </row>
     <row r="150" spans="1:31">
@@ -13430,7 +13487,7 @@
         <v>4</v>
       </c>
       <c r="B150" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C150" t="s">
         <v>193</v>
@@ -13439,40 +13496,40 @@
         <v>194</v>
       </c>
       <c r="T150">
-        <v>0.595</v>
+        <v>0.61907</v>
       </c>
       <c r="U150">
-        <v>0.521</v>
+        <v>1.15822</v>
       </c>
       <c r="V150">
-        <v>0.959</v>
+        <v>1.05779</v>
       </c>
       <c r="W150">
-        <v>0.748</v>
+        <v>1.00381</v>
       </c>
       <c r="X150">
-        <v>0.404</v>
+        <v>0.9641</v>
       </c>
       <c r="Y150">
-        <v>0.972</v>
+        <v>1.08885</v>
       </c>
       <c r="Z150">
-        <v>1.169</v>
+        <v>0.97573</v>
       </c>
       <c r="AA150">
-        <v>0.9460000000000001</v>
+        <v>1.11726</v>
       </c>
       <c r="AB150">
-        <v>0.7880799999999998</v>
+        <v>0.56872</v>
       </c>
       <c r="AC150">
-        <v>0.8164984079999998</v>
+        <v>0.4226284</v>
       </c>
       <c r="AD150">
-        <v>0.8534050686799997</v>
+        <v>0.519352314</v>
       </c>
       <c r="AE150">
-        <v>0.8881932261977996</v>
+        <v>0.50018883386</v>
       </c>
     </row>
     <row r="151" spans="1:31">
@@ -13480,7 +13537,7 @@
         <v>4</v>
       </c>
       <c r="B151" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C151" t="s">
         <v>193</v>
@@ -13489,85 +13546,85 @@
         <v>194</v>
       </c>
       <c r="E151">
-        <v>-1.27</v>
+        <v>-0.293</v>
       </c>
       <c r="F151">
-        <v>-1.524</v>
+        <v>-0.223</v>
       </c>
       <c r="G151">
-        <v>-2.2978</v>
+        <v>-0.236</v>
       </c>
       <c r="H151">
-        <v>-2.8219</v>
+        <v>-0.1227</v>
       </c>
       <c r="I151">
-        <v>-2.773</v>
+        <v>0.341</v>
       </c>
       <c r="J151">
-        <v>-3.0305</v>
+        <v>-0.1585</v>
       </c>
       <c r="K151">
-        <v>-3.075</v>
+        <v>-0.008</v>
       </c>
       <c r="L151">
-        <v>-3.0748</v>
+        <v>-0.2861</v>
       </c>
       <c r="M151">
-        <v>-2.7424</v>
+        <v>-0.4562</v>
       </c>
       <c r="N151">
-        <v>-3.198</v>
+        <v>-0.4378</v>
       </c>
       <c r="O151">
-        <v>-3.9897</v>
+        <v>-0.1267</v>
       </c>
       <c r="P151">
-        <v>-4.4644</v>
+        <v>-0.1167</v>
       </c>
       <c r="Q151">
-        <v>-4.5106</v>
+        <v>-0.3161</v>
       </c>
       <c r="R151">
-        <v>-4.59</v>
+        <v>-0.0056</v>
       </c>
       <c r="S151">
-        <v>-3.9447</v>
+        <v>-0.9816</v>
       </c>
       <c r="T151">
-        <v>-5.2088</v>
+        <v>-1.3049</v>
       </c>
       <c r="U151">
-        <v>-5.3024</v>
+        <v>-0.4657</v>
       </c>
       <c r="V151">
-        <v>-4.5547</v>
+        <v>-0.3087</v>
       </c>
       <c r="W151">
-        <v>-4.9039</v>
+        <v>-0.3754</v>
       </c>
       <c r="X151">
-        <v>-6.0074</v>
+        <v>2.684</v>
       </c>
       <c r="Y151">
-        <v>-6.7782</v>
+        <v>-0.2614</v>
       </c>
       <c r="Z151">
-        <v>-6.4232</v>
+        <v>-0.915</v>
       </c>
       <c r="AA151">
-        <v>-6.4025</v>
+        <v>0.0519</v>
       </c>
       <c r="AB151">
-        <v>-7.9044</v>
+        <v>0.4102</v>
       </c>
       <c r="AC151">
-        <v>-6.7732</v>
+        <v>0.3831</v>
       </c>
       <c r="AD151">
-        <v>0.8534050686799997</v>
+        <v>0.519352314</v>
       </c>
       <c r="AE151">
-        <v>0.8881932261977996</v>
+        <v>0.50018883386</v>
       </c>
     </row>
     <row r="152" spans="1:31">
@@ -13575,7 +13632,7 @@
         <v>4</v>
       </c>
       <c r="B152" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C152" t="s">
         <v>193</v>
@@ -13583,41 +13640,77 @@
       <c r="D152" t="s">
         <v>194</v>
       </c>
+      <c r="H152">
+        <v>0.08526</v>
+      </c>
+      <c r="I152">
+        <v>0.17276</v>
+      </c>
+      <c r="J152">
+        <v>0.17068</v>
+      </c>
+      <c r="K152">
+        <v>0.24678</v>
+      </c>
+      <c r="L152">
+        <v>0.22652</v>
+      </c>
+      <c r="M152">
+        <v>0.1417</v>
+      </c>
+      <c r="N152">
+        <v>0.21209</v>
+      </c>
+      <c r="O152">
+        <v>0.23732</v>
+      </c>
+      <c r="P152">
+        <v>0.26158</v>
+      </c>
+      <c r="Q152">
+        <v>0.36353</v>
+      </c>
+      <c r="R152">
+        <v>0.3176099999999999</v>
+      </c>
+      <c r="S152">
+        <v>0.42169</v>
+      </c>
       <c r="T152">
-        <v>0.61907</v>
+        <v>0.58136</v>
       </c>
       <c r="U152">
-        <v>1.15822</v>
+        <v>0.5704900000000001</v>
       </c>
       <c r="V152">
-        <v>1.05779</v>
+        <v>0.6081700000000001</v>
       </c>
       <c r="W152">
-        <v>1.00381</v>
+        <v>0.55608</v>
       </c>
       <c r="X152">
-        <v>0.9641</v>
+        <v>0.61771</v>
       </c>
       <c r="Y152">
-        <v>1.08885</v>
+        <v>0.70948</v>
       </c>
       <c r="Z152">
-        <v>0.97573</v>
+        <v>0.7603</v>
       </c>
       <c r="AA152">
-        <v>1.11726</v>
+        <v>0.76862</v>
       </c>
       <c r="AB152">
-        <v>0.56872</v>
+        <v>0.80028</v>
       </c>
       <c r="AC152">
-        <v>0.4226284</v>
+        <v>0.8202869999999999</v>
       </c>
       <c r="AD152">
-        <v>0.519352314</v>
+        <v>0.8407941749999998</v>
       </c>
       <c r="AE152">
-        <v>0.50018883386</v>
+        <v>0.8618140293749996</v>
       </c>
     </row>
     <row r="153" spans="1:31">
@@ -13625,7 +13718,7 @@
         <v>4</v>
       </c>
       <c r="B153" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C153" t="s">
         <v>193</v>
@@ -13633,86 +13726,80 @@
       <c r="D153" t="s">
         <v>194</v>
       </c>
-      <c r="E153">
-        <v>-0.293</v>
-      </c>
-      <c r="F153">
-        <v>-0.223</v>
-      </c>
       <c r="G153">
-        <v>-0.236</v>
+        <v>3.8766</v>
       </c>
       <c r="H153">
-        <v>-0.1227</v>
+        <v>4.096</v>
       </c>
       <c r="I153">
-        <v>0.341</v>
+        <v>4.3142</v>
       </c>
       <c r="J153">
-        <v>-0.1585</v>
+        <v>4.6072</v>
       </c>
       <c r="K153">
-        <v>-0.008</v>
+        <v>4.8688</v>
       </c>
       <c r="L153">
-        <v>-0.2861</v>
+        <v>4.934</v>
       </c>
       <c r="M153">
-        <v>-0.4562</v>
+        <v>5.394</v>
       </c>
       <c r="N153">
-        <v>-0.4378</v>
+        <v>6.0997</v>
       </c>
       <c r="O153">
-        <v>-0.1267</v>
+        <v>6.4395</v>
       </c>
       <c r="P153">
-        <v>-0.1167</v>
+        <v>6.8159</v>
       </c>
       <c r="Q153">
-        <v>-0.3161</v>
+        <v>7.345</v>
       </c>
       <c r="R153">
-        <v>-0.0056</v>
+        <v>7.626</v>
       </c>
       <c r="S153">
-        <v>-0.9816</v>
+        <v>7.8668</v>
       </c>
       <c r="T153">
-        <v>-1.3049</v>
+        <v>8.419499999999999</v>
       </c>
       <c r="U153">
-        <v>-0.4657</v>
+        <v>8.856199999999999</v>
       </c>
       <c r="V153">
-        <v>-0.3087</v>
+        <v>9.3468</v>
       </c>
       <c r="W153">
-        <v>-0.3754</v>
+        <v>9.939399999999999</v>
       </c>
       <c r="X153">
-        <v>2.684</v>
+        <v>10.1666</v>
       </c>
       <c r="Y153">
-        <v>-0.2614</v>
+        <v>10.7903</v>
       </c>
       <c r="Z153">
-        <v>-0.915</v>
+        <v>11.1216</v>
       </c>
       <c r="AA153">
-        <v>0.0519</v>
+        <v>11.2161</v>
       </c>
       <c r="AB153">
-        <v>0.4102</v>
+        <v>12.3329</v>
       </c>
       <c r="AC153">
-        <v>0.3831</v>
+        <v>12.8691</v>
       </c>
       <c r="AD153">
-        <v>0.519352314</v>
+        <v>0.8407941749999998</v>
       </c>
       <c r="AE153">
-        <v>0.50018883386</v>
+        <v>0.8618140293749996</v>
       </c>
     </row>
     <row r="154" spans="1:31">
@@ -13720,7 +13807,7 @@
         <v>4</v>
       </c>
       <c r="B154" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C154" t="s">
         <v>193</v>
@@ -13729,76 +13816,76 @@
         <v>194</v>
       </c>
       <c r="H154">
-        <v>0.08526</v>
+        <v>0.38789</v>
       </c>
       <c r="I154">
-        <v>0.17276</v>
+        <v>0.4263</v>
       </c>
       <c r="J154">
-        <v>0.17068</v>
+        <v>0.4396</v>
       </c>
       <c r="K154">
-        <v>0.24678</v>
+        <v>0.44393</v>
       </c>
       <c r="L154">
-        <v>0.22652</v>
+        <v>0.4497</v>
       </c>
       <c r="M154">
-        <v>0.1417</v>
+        <v>0.44792</v>
       </c>
       <c r="N154">
-        <v>0.21209</v>
+        <v>0.44373</v>
       </c>
       <c r="O154">
-        <v>0.23732</v>
+        <v>0.47165</v>
       </c>
       <c r="P154">
-        <v>0.26158</v>
+        <v>0.49576</v>
       </c>
       <c r="Q154">
-        <v>0.36353</v>
+        <v>0.54459</v>
       </c>
       <c r="R154">
-        <v>0.3176099999999999</v>
+        <v>0.6077</v>
       </c>
       <c r="S154">
-        <v>0.42169</v>
+        <v>0.7024600000000001</v>
       </c>
       <c r="T154">
-        <v>0.58136</v>
+        <v>0.8153899999999999</v>
       </c>
       <c r="U154">
-        <v>0.5704900000000001</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="V154">
-        <v>0.6081700000000001</v>
+        <v>0.81259</v>
       </c>
       <c r="W154">
-        <v>0.55608</v>
+        <v>0.88575</v>
       </c>
       <c r="X154">
-        <v>0.61771</v>
+        <v>0.9616399999999999</v>
       </c>
       <c r="Y154">
-        <v>0.70948</v>
+        <v>1.02627</v>
       </c>
       <c r="Z154">
-        <v>0.7603</v>
+        <v>1.07394</v>
       </c>
       <c r="AA154">
-        <v>0.76862</v>
+        <v>1.104</v>
       </c>
       <c r="AB154">
-        <v>0.80028</v>
+        <v>1.14178</v>
       </c>
       <c r="AC154">
-        <v>0.8202869999999999</v>
+        <v>1.1817423</v>
       </c>
       <c r="AD154">
-        <v>0.8407941749999998</v>
+        <v>1.229011992</v>
       </c>
       <c r="AE154">
-        <v>0.8618140293749996</v>
+        <v>1.27202741172</v>
       </c>
     </row>
     <row r="155" spans="1:31">
@@ -13806,7 +13893,7 @@
         <v>4</v>
       </c>
       <c r="B155" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C155" t="s">
         <v>193</v>
@@ -13815,79 +13902,79 @@
         <v>194</v>
       </c>
       <c r="G155">
-        <v>3.8766</v>
+        <v>4.7185</v>
       </c>
       <c r="H155">
-        <v>4.096</v>
+        <v>4.8239</v>
       </c>
       <c r="I155">
-        <v>4.3142</v>
+        <v>4.9175</v>
       </c>
       <c r="J155">
-        <v>4.6072</v>
+        <v>5.0739</v>
       </c>
       <c r="K155">
-        <v>4.8688</v>
+        <v>5.2345</v>
       </c>
       <c r="L155">
-        <v>4.934</v>
+        <v>5.4876</v>
       </c>
       <c r="M155">
-        <v>5.394</v>
+        <v>5.6321</v>
       </c>
       <c r="N155">
-        <v>6.0997</v>
+        <v>5.7755</v>
       </c>
       <c r="O155">
-        <v>6.4395</v>
+        <v>5.9971</v>
       </c>
       <c r="P155">
-        <v>6.8159</v>
+        <v>6.1106</v>
       </c>
       <c r="Q155">
-        <v>7.345</v>
+        <v>6.6167</v>
       </c>
       <c r="R155">
-        <v>7.626</v>
+        <v>7.12</v>
       </c>
       <c r="S155">
-        <v>7.8668</v>
+        <v>7.4704</v>
       </c>
       <c r="T155">
-        <v>8.419499999999999</v>
+        <v>7.8267</v>
       </c>
       <c r="U155">
-        <v>8.856199999999999</v>
+        <v>7.695</v>
       </c>
       <c r="V155">
-        <v>9.3468</v>
+        <v>8.073700000000001</v>
       </c>
       <c r="W155">
-        <v>9.939399999999999</v>
+        <v>8.585100000000001</v>
       </c>
       <c r="X155">
-        <v>10.1666</v>
+        <v>8.8848</v>
       </c>
       <c r="Y155">
-        <v>10.7903</v>
+        <v>8.992599999999999</v>
       </c>
       <c r="Z155">
-        <v>11.1216</v>
+        <v>9.0642</v>
       </c>
       <c r="AA155">
-        <v>11.2161</v>
+        <v>9.1327</v>
       </c>
       <c r="AB155">
-        <v>12.3329</v>
+        <v>9.2669</v>
       </c>
       <c r="AC155">
-        <v>12.8691</v>
+        <v>9.507</v>
       </c>
       <c r="AD155">
-        <v>0.8407941749999998</v>
+        <v>1.229011992</v>
       </c>
       <c r="AE155">
-        <v>0.8618140293749996</v>
+        <v>1.27202741172</v>
       </c>
     </row>
     <row r="156" spans="1:31">
@@ -13895,7 +13982,7 @@
         <v>4</v>
       </c>
       <c r="B156" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C156" t="s">
         <v>193</v>
@@ -13904,76 +13991,76 @@
         <v>194</v>
       </c>
       <c r="H156">
-        <v>0.38789</v>
+        <v>0.8373200000000001</v>
       </c>
       <c r="I156">
-        <v>0.4263</v>
+        <v>1.13032</v>
       </c>
       <c r="J156">
-        <v>0.4396</v>
+        <v>1.20863</v>
       </c>
       <c r="K156">
-        <v>0.44393</v>
+        <v>0.88362</v>
       </c>
       <c r="L156">
-        <v>0.4497</v>
+        <v>0.9705</v>
       </c>
       <c r="M156">
-        <v>0.44792</v>
+        <v>0.85673</v>
       </c>
       <c r="N156">
-        <v>0.44373</v>
+        <v>0.95312</v>
       </c>
       <c r="O156">
-        <v>0.47165</v>
+        <v>0.9871799999999999</v>
       </c>
       <c r="P156">
-        <v>0.49576</v>
+        <v>1.01808</v>
       </c>
       <c r="Q156">
-        <v>0.54459</v>
+        <v>1.16645</v>
       </c>
       <c r="R156">
-        <v>0.6077</v>
+        <v>1.39947</v>
       </c>
       <c r="S156">
-        <v>0.7024600000000001</v>
+        <v>1.48401</v>
       </c>
       <c r="T156">
-        <v>0.8153899999999999</v>
+        <v>1.81999</v>
       </c>
       <c r="U156">
-        <v>0.8169999999999999</v>
+        <v>1.52319</v>
       </c>
       <c r="V156">
-        <v>0.81259</v>
+        <v>1.75829</v>
       </c>
       <c r="W156">
-        <v>0.88575</v>
+        <v>1.58467</v>
       </c>
       <c r="X156">
-        <v>0.9616399999999999</v>
+        <v>1.64154</v>
       </c>
       <c r="Y156">
-        <v>1.02627</v>
+        <v>1.61977</v>
       </c>
       <c r="Z156">
-        <v>1.07394</v>
+        <v>1.70962</v>
       </c>
       <c r="AA156">
-        <v>1.104</v>
+        <v>1.86769</v>
       </c>
       <c r="AB156">
-        <v>1.14178</v>
+        <v>1.84643</v>
       </c>
       <c r="AC156">
-        <v>1.1817423</v>
+        <v>1.875400249273873</v>
       </c>
       <c r="AD156">
-        <v>1.229011992</v>
+        <v>2.013306546665499</v>
       </c>
       <c r="AE156">
-        <v>1.27202741172</v>
+        <v>2.11383160208286</v>
       </c>
     </row>
     <row r="157" spans="1:31">
@@ -13981,7 +14068,7 @@
         <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C157" t="s">
         <v>193</v>
@@ -13990,79 +14077,79 @@
         <v>194</v>
       </c>
       <c r="G157">
-        <v>4.7185</v>
+        <v>7.5193</v>
       </c>
       <c r="H157">
-        <v>4.8239</v>
+        <v>7.9761</v>
       </c>
       <c r="I157">
-        <v>4.9175</v>
+        <v>8.187999999999999</v>
       </c>
       <c r="J157">
-        <v>5.0739</v>
+        <v>8.556100000000001</v>
       </c>
       <c r="K157">
-        <v>5.2345</v>
+        <v>9.010899999999999</v>
       </c>
       <c r="L157">
-        <v>5.4876</v>
+        <v>9.4284</v>
       </c>
       <c r="M157">
-        <v>5.6321</v>
+        <v>9.988099999999999</v>
       </c>
       <c r="N157">
-        <v>5.7755</v>
+        <v>11.4903</v>
       </c>
       <c r="O157">
-        <v>5.9971</v>
+        <v>11.7447</v>
       </c>
       <c r="P157">
-        <v>6.1106</v>
+        <v>12.1379</v>
       </c>
       <c r="Q157">
-        <v>6.6167</v>
+        <v>12.4862</v>
       </c>
       <c r="R157">
-        <v>7.12</v>
+        <v>12.8621</v>
       </c>
       <c r="S157">
-        <v>7.4704</v>
+        <v>12.9176</v>
       </c>
       <c r="T157">
-        <v>7.8267</v>
+        <v>14.0088</v>
       </c>
       <c r="U157">
-        <v>7.695</v>
+        <v>15.0093</v>
       </c>
       <c r="V157">
-        <v>8.073700000000001</v>
+        <v>15.1658</v>
       </c>
       <c r="W157">
-        <v>8.585100000000001</v>
+        <v>15.8702</v>
       </c>
       <c r="X157">
-        <v>8.8848</v>
+        <v>16.4953</v>
       </c>
       <c r="Y157">
-        <v>8.992599999999999</v>
+        <v>17.0939</v>
       </c>
       <c r="Z157">
-        <v>9.0642</v>
+        <v>16.9955</v>
       </c>
       <c r="AA157">
-        <v>9.1327</v>
+        <v>16.6931</v>
       </c>
       <c r="AB157">
-        <v>9.2669</v>
+        <v>16.7587</v>
       </c>
       <c r="AC157">
-        <v>9.507</v>
+        <v>17.6226</v>
       </c>
       <c r="AD157">
-        <v>1.229011992</v>
+        <v>2.013306546665499</v>
       </c>
       <c r="AE157">
-        <v>1.27202741172</v>
+        <v>2.11383160208286</v>
       </c>
     </row>
     <row r="158" spans="1:31">
@@ -14070,7 +14157,7 @@
         <v>4</v>
       </c>
       <c r="B158" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C158" t="s">
         <v>193</v>
@@ -14079,76 +14166,76 @@
         <v>194</v>
       </c>
       <c r="H158">
-        <v>0.8373200000000001</v>
+        <v>0.17881</v>
       </c>
       <c r="I158">
-        <v>1.13032</v>
+        <v>0.14405</v>
       </c>
       <c r="J158">
-        <v>1.20863</v>
+        <v>0.23977</v>
       </c>
       <c r="K158">
-        <v>0.88362</v>
+        <v>0.22492</v>
       </c>
       <c r="L158">
-        <v>0.9705</v>
+        <v>0.18768</v>
       </c>
       <c r="M158">
-        <v>0.85673</v>
+        <v>0.18218</v>
       </c>
       <c r="N158">
-        <v>0.95312</v>
+        <v>0.21963</v>
       </c>
       <c r="O158">
-        <v>0.9871799999999999</v>
+        <v>0.24327</v>
       </c>
       <c r="P158">
-        <v>1.01808</v>
+        <v>0.26491</v>
       </c>
       <c r="Q158">
-        <v>1.16645</v>
+        <v>0.38077</v>
       </c>
       <c r="R158">
-        <v>1.39947</v>
+        <v>0.40255</v>
       </c>
       <c r="S158">
-        <v>1.48401</v>
+        <v>0.45736</v>
       </c>
       <c r="T158">
-        <v>1.81999</v>
+        <v>0.5645</v>
       </c>
       <c r="U158">
-        <v>1.52319</v>
+        <v>0.5366299999999999</v>
       </c>
       <c r="V158">
-        <v>1.75829</v>
+        <v>0.53662</v>
       </c>
       <c r="W158">
-        <v>1.58467</v>
+        <v>0.6198400000000001</v>
       </c>
       <c r="X158">
-        <v>1.64154</v>
+        <v>0.58473</v>
       </c>
       <c r="Y158">
-        <v>1.61977</v>
+        <v>0.55326</v>
       </c>
       <c r="Z158">
-        <v>1.70962</v>
+        <v>0.57773</v>
       </c>
       <c r="AA158">
-        <v>1.86769</v>
+        <v>0.6183</v>
       </c>
       <c r="AB158">
-        <v>1.84643</v>
+        <v>0.6426900000000001</v>
       </c>
       <c r="AC158">
-        <v>1.875400249273873</v>
+        <v>0.6651841500000001</v>
       </c>
       <c r="AD158">
-        <v>2.013306546665499</v>
+        <v>0.6884655952500001</v>
       </c>
       <c r="AE158">
-        <v>2.11383160208286</v>
+        <v>0.7091195631075001</v>
       </c>
     </row>
     <row r="159" spans="1:31">
@@ -14156,7 +14243,7 @@
         <v>4</v>
       </c>
       <c r="B159" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C159" t="s">
         <v>193</v>
@@ -14165,79 +14252,79 @@
         <v>194</v>
       </c>
       <c r="G159">
-        <v>7.5193</v>
+        <v>12.0749</v>
       </c>
       <c r="H159">
-        <v>7.9761</v>
+        <v>12.9524</v>
       </c>
       <c r="I159">
-        <v>8.187999999999999</v>
+        <v>12.9475</v>
       </c>
       <c r="J159">
-        <v>8.556100000000001</v>
+        <v>13.5101</v>
       </c>
       <c r="K159">
-        <v>9.010899999999999</v>
+        <v>14.3796</v>
       </c>
       <c r="L159">
-        <v>9.4284</v>
+        <v>15.3498</v>
       </c>
       <c r="M159">
-        <v>9.988099999999999</v>
+        <v>16.4805</v>
       </c>
       <c r="N159">
-        <v>11.4903</v>
+        <v>17.0678</v>
       </c>
       <c r="O159">
-        <v>11.7447</v>
+        <v>18.5125</v>
       </c>
       <c r="P159">
-        <v>12.1379</v>
+        <v>20.0596</v>
       </c>
       <c r="Q159">
-        <v>12.4862</v>
+        <v>21.032</v>
       </c>
       <c r="R159">
-        <v>12.8621</v>
+        <v>21.5001</v>
       </c>
       <c r="S159">
-        <v>12.9176</v>
+        <v>22.6581</v>
       </c>
       <c r="T159">
-        <v>14.0088</v>
+        <v>24.9802</v>
       </c>
       <c r="U159">
-        <v>15.0093</v>
+        <v>26.6927</v>
       </c>
       <c r="V159">
-        <v>15.1658</v>
+        <v>27.7283</v>
       </c>
       <c r="W159">
-        <v>15.8702</v>
+        <v>29.3849</v>
       </c>
       <c r="X159">
-        <v>16.4953</v>
+        <v>30.7127</v>
       </c>
       <c r="Y159">
-        <v>17.0939</v>
+        <v>31.1827</v>
       </c>
       <c r="Z159">
-        <v>16.9955</v>
+        <v>32.1192</v>
       </c>
       <c r="AA159">
-        <v>16.6931</v>
+        <v>32.8825</v>
       </c>
       <c r="AB159">
-        <v>16.7587</v>
+        <v>33.738</v>
       </c>
       <c r="AC159">
-        <v>17.6226</v>
+        <v>34.8742</v>
       </c>
       <c r="AD159">
-        <v>2.013306546665499</v>
+        <v>0.6884655952500001</v>
       </c>
       <c r="AE159">
-        <v>2.11383160208286</v>
+        <v>0.7091195631075001</v>
       </c>
     </row>
     <row r="160" spans="1:31">
@@ -14245,7 +14332,7 @@
         <v>4</v>
       </c>
       <c r="B160" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C160" t="s">
         <v>193</v>
@@ -14253,77 +14340,68 @@
       <c r="D160" t="s">
         <v>194</v>
       </c>
-      <c r="H160">
-        <v>0.17881</v>
-      </c>
-      <c r="I160">
-        <v>0.14405</v>
-      </c>
-      <c r="J160">
-        <v>0.23977</v>
-      </c>
       <c r="K160">
-        <v>0.22492</v>
+        <v>2.354947567308822</v>
       </c>
       <c r="L160">
-        <v>0.18768</v>
+        <v>3.084524636867933</v>
       </c>
       <c r="M160">
-        <v>0.18218</v>
+        <v>3.637483315174352</v>
       </c>
       <c r="N160">
-        <v>0.21963</v>
+        <v>3.846776048053812</v>
       </c>
       <c r="O160">
-        <v>0.24327</v>
+        <v>3.869343308269463</v>
       </c>
       <c r="P160">
-        <v>0.26491</v>
+        <v>5.029789426923946</v>
       </c>
       <c r="Q160">
-        <v>0.38077</v>
+        <v>6.237199297303407</v>
       </c>
       <c r="R160">
-        <v>0.40255</v>
+        <v>7.174499999999999</v>
       </c>
       <c r="S160">
-        <v>0.45736</v>
+        <v>8.110900000000001</v>
       </c>
       <c r="T160">
-        <v>0.5645</v>
+        <v>9.7027</v>
       </c>
       <c r="U160">
-        <v>0.5366299999999999</v>
+        <v>7.5919</v>
       </c>
       <c r="V160">
-        <v>0.53662</v>
+        <v>9.553700000000001</v>
       </c>
       <c r="W160">
-        <v>0.6198400000000001</v>
+        <v>12.3715</v>
       </c>
       <c r="X160">
-        <v>0.58473</v>
+        <v>13.9255</v>
       </c>
       <c r="Y160">
-        <v>0.55326</v>
+        <v>13.6123</v>
       </c>
       <c r="Z160">
-        <v>0.57773</v>
+        <v>13.3583</v>
       </c>
       <c r="AA160">
-        <v>0.6183</v>
+        <v>14.0489</v>
       </c>
       <c r="AB160">
-        <v>0.6426900000000001</v>
+        <v>13.721</v>
       </c>
       <c r="AC160">
-        <v>0.6651841500000001</v>
+        <v>15.371</v>
       </c>
       <c r="AD160">
-        <v>0.6884655952500001</v>
+        <v>17.65946544734863</v>
       </c>
       <c r="AE160">
-        <v>0.7091195631075001</v>
+        <v>18.92770997069262</v>
       </c>
     </row>
     <row r="161" spans="1:31">
@@ -14331,7 +14409,7 @@
         <v>4</v>
       </c>
       <c r="B161" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C161" t="s">
         <v>193</v>
@@ -14339,80 +14417,86 @@
       <c r="D161" t="s">
         <v>194</v>
       </c>
+      <c r="E161">
+        <v>80.13113771</v>
+      </c>
+      <c r="F161">
+        <v>85.9837589</v>
+      </c>
       <c r="G161">
-        <v>12.0749</v>
+        <v>94.41824505</v>
       </c>
       <c r="H161">
-        <v>12.9524</v>
+        <v>100.6597388</v>
       </c>
       <c r="I161">
-        <v>12.9475</v>
+        <v>111.5890644</v>
       </c>
       <c r="J161">
-        <v>13.5101</v>
+        <v>122.2627749</v>
       </c>
       <c r="K161">
-        <v>14.3796</v>
+        <v>132.4104</v>
       </c>
       <c r="L161">
-        <v>15.3498</v>
+        <v>156.6955</v>
       </c>
       <c r="M161">
-        <v>16.4805</v>
+        <v>165.806</v>
       </c>
       <c r="N161">
-        <v>17.0678</v>
+        <v>172.6238</v>
       </c>
       <c r="O161">
-        <v>18.5125</v>
+        <v>174.6047</v>
       </c>
       <c r="P161">
-        <v>20.0596</v>
+        <v>190.2729</v>
       </c>
       <c r="Q161">
-        <v>21.032</v>
+        <v>206.456</v>
       </c>
       <c r="R161">
-        <v>21.5001</v>
+        <v>223.3871</v>
       </c>
       <c r="S161">
-        <v>22.6581</v>
+        <v>239.4861</v>
       </c>
       <c r="T161">
-        <v>24.9802</v>
+        <v>246.8437</v>
       </c>
       <c r="U161">
-        <v>26.6927</v>
+        <v>201.2788</v>
       </c>
       <c r="V161">
-        <v>27.7283</v>
+        <v>224.5962</v>
       </c>
       <c r="W161">
-        <v>29.3849</v>
+        <v>246.0418</v>
       </c>
       <c r="X161">
-        <v>30.7127</v>
+        <v>243.051</v>
       </c>
       <c r="Y161">
-        <v>31.1827</v>
+        <v>247.5724</v>
       </c>
       <c r="Z161">
-        <v>32.1192</v>
+        <v>250.5964</v>
       </c>
       <c r="AA161">
-        <v>32.8825</v>
+        <v>256.4936</v>
       </c>
       <c r="AB161">
-        <v>33.738</v>
+        <v>258.7764</v>
       </c>
       <c r="AC161">
-        <v>34.8742</v>
+        <v>274.4643</v>
       </c>
       <c r="AD161">
-        <v>0.6884655952500001</v>
+        <v>17.65946544734863</v>
       </c>
       <c r="AE161">
-        <v>0.7091195631075001</v>
+        <v>18.92770997069262</v>
       </c>
     </row>
     <row r="162" spans="1:31">
@@ -14420,7 +14504,7 @@
         <v>4</v>
       </c>
       <c r="B162" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C162" t="s">
         <v>193</v>
@@ -14428,68 +14512,77 @@
       <c r="D162" t="s">
         <v>194</v>
       </c>
+      <c r="H162">
+        <v>0</v>
+      </c>
+      <c r="I162">
+        <v>0</v>
+      </c>
+      <c r="J162">
+        <v>0</v>
+      </c>
       <c r="K162">
-        <v>2.354947567308822</v>
+        <v>0</v>
       </c>
       <c r="L162">
-        <v>3.084524636867933</v>
+        <v>0.03851</v>
       </c>
       <c r="M162">
-        <v>3.637483315174352</v>
+        <v>0.04568</v>
       </c>
       <c r="N162">
-        <v>3.846776048053812</v>
+        <v>0.02674</v>
       </c>
       <c r="O162">
-        <v>3.869343308269463</v>
+        <v>0.01432</v>
       </c>
       <c r="P162">
-        <v>5.029789426923946</v>
+        <v>0.01199</v>
       </c>
       <c r="Q162">
-        <v>6.237199297303407</v>
+        <v>0.009800000000000001</v>
       </c>
       <c r="R162">
-        <v>7.174499999999999</v>
+        <v>0.01498</v>
       </c>
       <c r="S162">
-        <v>8.110900000000001</v>
+        <v>0.0089</v>
       </c>
       <c r="T162">
-        <v>9.7027</v>
+        <v>0.01867</v>
       </c>
       <c r="U162">
-        <v>7.5919</v>
+        <v>0.04725</v>
       </c>
       <c r="V162">
-        <v>9.553700000000001</v>
+        <v>0.03195</v>
       </c>
       <c r="W162">
-        <v>12.3715</v>
+        <v>0.01594</v>
       </c>
       <c r="X162">
-        <v>13.9255</v>
+        <v>0.01412</v>
       </c>
       <c r="Y162">
-        <v>13.6123</v>
+        <v>0.01741</v>
       </c>
       <c r="Z162">
-        <v>13.3583</v>
+        <v>0.01514</v>
       </c>
       <c r="AA162">
-        <v>14.0489</v>
+        <v>0.01763</v>
       </c>
       <c r="AB162">
-        <v>13.721</v>
+        <v>0.01421</v>
       </c>
       <c r="AC162">
-        <v>15.371</v>
+        <v>0.01421</v>
       </c>
       <c r="AD162">
-        <v>17.65946544734863</v>
+        <v>0.01421</v>
       </c>
       <c r="AE162">
-        <v>18.92770997069262</v>
+        <v>0.01421</v>
       </c>
     </row>
     <row r="163" spans="1:31">
@@ -14497,7 +14590,7 @@
         <v>4</v>
       </c>
       <c r="B163" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C163" t="s">
         <v>193</v>
@@ -14505,86 +14598,80 @@
       <c r="D163" t="s">
         <v>194</v>
       </c>
-      <c r="E163">
-        <v>80.13113771</v>
-      </c>
-      <c r="F163">
-        <v>85.9837589</v>
-      </c>
       <c r="G163">
-        <v>94.41824505</v>
+        <v>0</v>
       </c>
       <c r="H163">
-        <v>100.6597388</v>
+        <v>0</v>
       </c>
       <c r="I163">
-        <v>111.5890644</v>
+        <v>0</v>
       </c>
       <c r="J163">
-        <v>122.2627749</v>
+        <v>0</v>
       </c>
       <c r="K163">
-        <v>132.4104</v>
+        <v>0</v>
       </c>
       <c r="L163">
-        <v>156.6955</v>
+        <v>0</v>
       </c>
       <c r="M163">
-        <v>165.806</v>
+        <v>0</v>
       </c>
       <c r="N163">
-        <v>172.6238</v>
+        <v>0</v>
       </c>
       <c r="O163">
-        <v>174.6047</v>
+        <v>0</v>
       </c>
       <c r="P163">
-        <v>190.2729</v>
+        <v>0</v>
       </c>
       <c r="Q163">
-        <v>206.456</v>
+        <v>0</v>
       </c>
       <c r="R163">
-        <v>223.3871</v>
+        <v>0</v>
       </c>
       <c r="S163">
-        <v>239.4861</v>
+        <v>0</v>
       </c>
       <c r="T163">
-        <v>246.8437</v>
+        <v>0</v>
       </c>
       <c r="U163">
-        <v>201.2788</v>
+        <v>0</v>
       </c>
       <c r="V163">
-        <v>224.5962</v>
+        <v>0</v>
       </c>
       <c r="W163">
-        <v>246.0418</v>
+        <v>0</v>
       </c>
       <c r="X163">
-        <v>243.051</v>
+        <v>0</v>
       </c>
       <c r="Y163">
-        <v>247.5724</v>
+        <v>0</v>
       </c>
       <c r="Z163">
-        <v>250.5964</v>
+        <v>0</v>
       </c>
       <c r="AA163">
-        <v>256.4936</v>
+        <v>0</v>
       </c>
       <c r="AB163">
-        <v>258.7764</v>
+        <v>0</v>
       </c>
       <c r="AC163">
-        <v>274.4643</v>
+        <v>0</v>
       </c>
       <c r="AD163">
-        <v>17.65946544734863</v>
+        <v>0</v>
       </c>
       <c r="AE163">
-        <v>18.92770997069262</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:31">
@@ -14592,7 +14679,7 @@
         <v>4</v>
       </c>
       <c r="B164" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C164" t="s">
         <v>193</v>
@@ -14600,77 +14687,68 @@
       <c r="D164" t="s">
         <v>194</v>
       </c>
-      <c r="H164">
-        <v>0</v>
-      </c>
-      <c r="I164">
-        <v>0</v>
-      </c>
-      <c r="J164">
-        <v>0</v>
-      </c>
       <c r="K164">
-        <v>0</v>
+        <v>0.8365627364282321</v>
       </c>
       <c r="L164">
-        <v>0.03851</v>
+        <v>1.040874561729843</v>
       </c>
       <c r="M164">
-        <v>0.04568</v>
+        <v>1.322815523915373</v>
       </c>
       <c r="N164">
-        <v>0.02674</v>
+        <v>1.70046056903603</v>
       </c>
       <c r="O164">
-        <v>0.01432</v>
+        <v>2.288766466110288</v>
       </c>
       <c r="P164">
-        <v>0.01199</v>
+        <v>2.448243528440106</v>
       </c>
       <c r="Q164">
-        <v>0.009800000000000001</v>
+        <v>3.252699633543705</v>
       </c>
       <c r="R164">
-        <v>0.01498</v>
+        <v>4.088200000000001</v>
       </c>
       <c r="S164">
-        <v>0.0089</v>
+        <v>4.3987</v>
       </c>
       <c r="T164">
-        <v>0.01867</v>
+        <v>6.374400000000001</v>
       </c>
       <c r="U164">
-        <v>0.04725</v>
+        <v>4.205100000000002</v>
       </c>
       <c r="V164">
-        <v>0.03195</v>
+        <v>6.097299999999998</v>
       </c>
       <c r="W164">
-        <v>0.01594</v>
+        <v>7.779600000000001</v>
       </c>
       <c r="X164">
-        <v>0.01412</v>
+        <v>9.121900000000002</v>
       </c>
       <c r="Y164">
-        <v>0.01741</v>
+        <v>10.9321</v>
       </c>
       <c r="Z164">
-        <v>0.01514</v>
+        <v>11.0028</v>
       </c>
       <c r="AA164">
-        <v>0.01763</v>
+        <v>8.855500000000005</v>
       </c>
       <c r="AB164">
-        <v>0.01421</v>
+        <v>8.886200000000001</v>
       </c>
       <c r="AC164">
-        <v>0.01421</v>
+        <v>11.0702</v>
       </c>
       <c r="AD164">
-        <v>0.01421</v>
+        <v>12.39862400000001</v>
       </c>
       <c r="AE164">
-        <v>0.01421</v>
+        <v>13.08054832000001</v>
       </c>
     </row>
     <row r="165" spans="1:31">
@@ -14678,7 +14756,7 @@
         <v>4</v>
       </c>
       <c r="B165" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C165" t="s">
         <v>193</v>
@@ -14686,80 +14764,86 @@
       <c r="D165" t="s">
         <v>194</v>
       </c>
+      <c r="E165">
+        <v>21.8066566</v>
+      </c>
+      <c r="F165">
+        <v>32.24145314</v>
+      </c>
       <c r="G165">
-        <v>0</v>
+        <v>32.05441746</v>
       </c>
       <c r="H165">
-        <v>0</v>
+        <v>30.80770017</v>
       </c>
       <c r="I165">
-        <v>0</v>
+        <v>43.35801110000001</v>
       </c>
       <c r="J165">
-        <v>0</v>
+        <v>41.69795026</v>
       </c>
       <c r="K165">
-        <v>0</v>
+        <v>35.6808</v>
       </c>
       <c r="L165">
-        <v>0</v>
+        <v>47.2577</v>
       </c>
       <c r="M165">
-        <v>0</v>
+        <v>46.7315</v>
       </c>
       <c r="N165">
-        <v>0</v>
+        <v>55.9374</v>
       </c>
       <c r="O165">
-        <v>0</v>
+        <v>51.3649</v>
       </c>
       <c r="P165">
-        <v>0</v>
+        <v>56.4241</v>
       </c>
       <c r="Q165">
-        <v>0</v>
+        <v>62.3327</v>
       </c>
       <c r="R165">
-        <v>0</v>
+        <v>68.7</v>
       </c>
       <c r="S165">
-        <v>0</v>
+        <v>74.9627</v>
       </c>
       <c r="T165">
-        <v>0</v>
+        <v>73.96129999999999</v>
       </c>
       <c r="U165">
-        <v>0</v>
+        <v>64.7072</v>
       </c>
       <c r="V165">
-        <v>0</v>
+        <v>82.9337</v>
       </c>
       <c r="W165">
-        <v>0</v>
+        <v>95.6763</v>
       </c>
       <c r="X165">
-        <v>0</v>
+        <v>104.0372</v>
       </c>
       <c r="Y165">
-        <v>0</v>
+        <v>105.3832</v>
       </c>
       <c r="Z165">
-        <v>0</v>
+        <v>104.6913</v>
       </c>
       <c r="AA165">
-        <v>0</v>
+        <v>101.2598</v>
       </c>
       <c r="AB165">
-        <v>0</v>
+        <v>100.7673</v>
       </c>
       <c r="AC165">
-        <v>0</v>
+        <v>106.5562</v>
       </c>
       <c r="AD165">
-        <v>0</v>
+        <v>12.39862400000001</v>
       </c>
       <c r="AE165">
-        <v>0</v>
+        <v>13.08054832000001</v>
       </c>
     </row>
     <row r="166" spans="1:31">
@@ -14767,7 +14851,7 @@
         <v>4</v>
       </c>
       <c r="B166" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C166" t="s">
         <v>193</v>
@@ -14776,67 +14860,67 @@
         <v>194</v>
       </c>
       <c r="K166">
-        <v>0.8365627364282321</v>
+        <v>3.240785256768478</v>
       </c>
       <c r="L166">
-        <v>1.040874561729843</v>
+        <v>3.335165005320667</v>
       </c>
       <c r="M166">
-        <v>1.322815523915373</v>
+        <v>3.848407547340623</v>
       </c>
       <c r="N166">
-        <v>1.70046056903603</v>
+        <v>4.5366989492076</v>
       </c>
       <c r="O166">
-        <v>2.288766466110288</v>
+        <v>4.786329873029657</v>
       </c>
       <c r="P166">
-        <v>2.448243528440106</v>
+        <v>6.327912506847197</v>
       </c>
       <c r="Q166">
-        <v>3.252699633543705</v>
+        <v>7.437099162120049</v>
       </c>
       <c r="R166">
-        <v>4.088200000000001</v>
+        <v>9.687299999999999</v>
       </c>
       <c r="S166">
-        <v>4.3987</v>
+        <v>12.1796</v>
       </c>
       <c r="T166">
-        <v>6.374400000000001</v>
+        <v>12.1737</v>
       </c>
       <c r="U166">
-        <v>4.205100000000002</v>
+        <v>7.7571</v>
       </c>
       <c r="V166">
-        <v>6.097299999999998</v>
+        <v>9.993399999999999</v>
       </c>
       <c r="W166">
-        <v>7.779600000000001</v>
+        <v>12.9548</v>
       </c>
       <c r="X166">
-        <v>9.121900000000002</v>
+        <v>14.3413</v>
       </c>
       <c r="Y166">
-        <v>10.9321</v>
+        <v>15.8088</v>
       </c>
       <c r="Z166">
-        <v>11.0028</v>
+        <v>16.9823</v>
       </c>
       <c r="AA166">
-        <v>8.855500000000005</v>
+        <v>17.1987</v>
       </c>
       <c r="AB166">
-        <v>8.886200000000001</v>
+        <v>17.5396</v>
       </c>
       <c r="AC166">
-        <v>11.0702</v>
+        <v>20.1161</v>
       </c>
       <c r="AD166">
-        <v>12.39862400000001</v>
+        <v>21.73730879371184</v>
       </c>
       <c r="AE166">
-        <v>13.08054832000001</v>
+        <v>23.1912167488825</v>
       </c>
     </row>
     <row r="167" spans="1:31">
@@ -14844,7 +14928,7 @@
         <v>4</v>
       </c>
       <c r="B167" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C167" t="s">
         <v>193</v>
@@ -14853,85 +14937,85 @@
         <v>194</v>
       </c>
       <c r="E167">
-        <v>21.8066566</v>
+        <v>67.54348644</v>
       </c>
       <c r="F167">
-        <v>32.24145314</v>
+        <v>72.36037648</v>
       </c>
       <c r="G167">
-        <v>32.05441746</v>
+        <v>79.07341540000002</v>
       </c>
       <c r="H167">
-        <v>30.80770017</v>
+        <v>86.56758657</v>
       </c>
       <c r="I167">
-        <v>43.35801110000001</v>
+        <v>95.31723175</v>
       </c>
       <c r="J167">
-        <v>41.69795026</v>
+        <v>102.7766112</v>
       </c>
       <c r="K167">
-        <v>35.6808</v>
+        <v>111.8473</v>
       </c>
       <c r="L167">
-        <v>47.2577</v>
+        <v>136.2034</v>
       </c>
       <c r="M167">
-        <v>46.7315</v>
+        <v>143.6356</v>
       </c>
       <c r="N167">
-        <v>55.9374</v>
+        <v>152.8791</v>
       </c>
       <c r="O167">
-        <v>51.3649</v>
+        <v>152.8528</v>
       </c>
       <c r="P167">
-        <v>56.4241</v>
+        <v>167.285</v>
       </c>
       <c r="Q167">
-        <v>62.3327</v>
+        <v>184.7259</v>
       </c>
       <c r="R167">
-        <v>68.7</v>
+        <v>200.1485</v>
       </c>
       <c r="S167">
-        <v>74.9627</v>
+        <v>211.9428</v>
       </c>
       <c r="T167">
-        <v>73.96129999999999</v>
+        <v>221.6384</v>
       </c>
       <c r="U167">
-        <v>64.7072</v>
+        <v>178.9665</v>
       </c>
       <c r="V167">
-        <v>82.9337</v>
+        <v>203.9589</v>
       </c>
       <c r="W167">
-        <v>95.6763</v>
+        <v>227.0114</v>
       </c>
       <c r="X167">
-        <v>104.0372</v>
+        <v>230.9442</v>
       </c>
       <c r="Y167">
-        <v>105.3832</v>
+        <v>225.9079</v>
       </c>
       <c r="Z167">
-        <v>104.6913</v>
+        <v>221.7976</v>
       </c>
       <c r="AA167">
-        <v>101.2598</v>
+        <v>212.5685</v>
       </c>
       <c r="AB167">
-        <v>100.7673</v>
+        <v>218.5098</v>
       </c>
       <c r="AC167">
-        <v>106.5562</v>
+        <v>231.5443</v>
       </c>
       <c r="AD167">
-        <v>12.39862400000001</v>
+        <v>21.73730879371184</v>
       </c>
       <c r="AE167">
-        <v>13.08054832000001</v>
+        <v>23.1912167488825</v>
       </c>
     </row>
     <row r="168" spans="1:31">
@@ -14939,7 +15023,7 @@
         <v>4</v>
       </c>
       <c r="B168" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C168" t="s">
         <v>193</v>
@@ -14948,67 +15032,67 @@
         <v>194</v>
       </c>
       <c r="K168">
-        <v>3.240785256768478</v>
+        <v>2.130555112025372</v>
       </c>
       <c r="L168">
-        <v>3.335165005320667</v>
+        <v>2.744736776134615</v>
       </c>
       <c r="M168">
-        <v>3.848407547340623</v>
+        <v>3.176209760717272</v>
       </c>
       <c r="N168">
-        <v>4.5366989492076</v>
+        <v>3.436990299329008</v>
       </c>
       <c r="O168">
-        <v>4.786329873029657</v>
+        <v>3.739345212938138</v>
       </c>
       <c r="P168">
-        <v>6.327912506847197</v>
+        <v>3.630564549465651</v>
       </c>
       <c r="Q168">
-        <v>7.437099162120049</v>
+        <v>5.060599429861737</v>
       </c>
       <c r="R168">
-        <v>9.687299999999999</v>
+        <v>5.7422</v>
       </c>
       <c r="S168">
-        <v>12.1796</v>
+        <v>5.633099999999999</v>
       </c>
       <c r="T168">
-        <v>12.1737</v>
+        <v>8.9702</v>
       </c>
       <c r="U168">
-        <v>7.7571</v>
+        <v>5.365799999999998</v>
       </c>
       <c r="V168">
-        <v>9.993399999999999</v>
+        <v>7.659800000000001</v>
       </c>
       <c r="W168">
-        <v>12.9548</v>
+        <v>9.871000000000002</v>
       </c>
       <c r="X168">
-        <v>14.3413</v>
+        <v>10.5376</v>
       </c>
       <c r="Y168">
-        <v>15.8088</v>
+        <v>10.3989</v>
       </c>
       <c r="Z168">
-        <v>16.9823</v>
+        <v>8.907200000000001</v>
       </c>
       <c r="AA168">
-        <v>17.1987</v>
+        <v>8.200900000000001</v>
       </c>
       <c r="AB168">
-        <v>17.5396</v>
+        <v>7.159900000000001</v>
       </c>
       <c r="AC168">
-        <v>20.1161</v>
+        <v>8.679700000000004</v>
       </c>
       <c r="AD168">
-        <v>21.73730879371184</v>
+        <v>9.721264000000005</v>
       </c>
       <c r="AE168">
-        <v>23.1912167488825</v>
+        <v>10.40175248000001</v>
       </c>
     </row>
     <row r="169" spans="1:31">
@@ -15016,7 +15100,7 @@
         <v>4</v>
       </c>
       <c r="B169" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C169" t="s">
         <v>193</v>
@@ -15025,85 +15109,85 @@
         <v>194</v>
       </c>
       <c r="E169">
-        <v>67.54348644</v>
+        <v>27.39165513</v>
       </c>
       <c r="F169">
-        <v>72.36037648</v>
+        <v>34.29965429999999</v>
       </c>
       <c r="G169">
-        <v>79.07341540000002</v>
+        <v>33.67331613</v>
       </c>
       <c r="H169">
-        <v>86.56758657</v>
+        <v>33.47762618</v>
       </c>
       <c r="I169">
-        <v>95.31723175</v>
+        <v>48.65726483</v>
       </c>
       <c r="J169">
-        <v>102.7766112</v>
+        <v>48.89512829</v>
       </c>
       <c r="K169">
-        <v>111.8473</v>
+        <v>42.7878</v>
       </c>
       <c r="L169">
-        <v>136.2034</v>
+        <v>55.9915</v>
       </c>
       <c r="M169">
-        <v>143.6356</v>
+        <v>55.8556</v>
       </c>
       <c r="N169">
-        <v>152.8791</v>
+        <v>56.8408</v>
       </c>
       <c r="O169">
-        <v>152.8528</v>
+        <v>54.8424</v>
       </c>
       <c r="P169">
-        <v>167.285</v>
+        <v>62.3321</v>
       </c>
       <c r="Q169">
-        <v>184.7259</v>
+        <v>71.443</v>
       </c>
       <c r="R169">
-        <v>200.1485</v>
+        <v>79.90470000000001</v>
       </c>
       <c r="S169">
-        <v>211.9428</v>
+        <v>88.3548</v>
       </c>
       <c r="T169">
-        <v>221.6384</v>
+        <v>95.405</v>
       </c>
       <c r="U169">
-        <v>178.9665</v>
+        <v>75.40100000000001</v>
       </c>
       <c r="V169">
-        <v>203.9589</v>
+        <v>91.1133</v>
       </c>
       <c r="W169">
-        <v>227.0114</v>
+        <v>108.4361</v>
       </c>
       <c r="X169">
-        <v>230.9442</v>
+        <v>110.8431</v>
       </c>
       <c r="Y169">
-        <v>225.9079</v>
+        <v>114.1851</v>
       </c>
       <c r="Z169">
-        <v>221.7976</v>
+        <v>119.6292</v>
       </c>
       <c r="AA169">
-        <v>212.5685</v>
+        <v>126.0022</v>
       </c>
       <c r="AB169">
-        <v>218.5098</v>
+        <v>123.9707</v>
       </c>
       <c r="AC169">
-        <v>231.5443</v>
+        <v>128.6282</v>
       </c>
       <c r="AD169">
-        <v>21.73730879371184</v>
+        <v>9.721264000000005</v>
       </c>
       <c r="AE169">
-        <v>23.1912167488825</v>
+        <v>10.40175248000001</v>
       </c>
     </row>
     <row r="170" spans="1:31">
@@ -15111,7 +15195,7 @@
         <v>4</v>
       </c>
       <c r="B170" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C170" t="s">
         <v>193</v>
@@ -15119,68 +15203,23 @@
       <c r="D170" t="s">
         <v>194</v>
       </c>
-      <c r="K170">
-        <v>2.130555112025372</v>
-      </c>
-      <c r="L170">
-        <v>2.744736776134615</v>
-      </c>
-      <c r="M170">
-        <v>3.176209760717272</v>
-      </c>
-      <c r="N170">
-        <v>3.436990299329008</v>
-      </c>
-      <c r="O170">
-        <v>3.739345212938138</v>
-      </c>
-      <c r="P170">
-        <v>3.630564549465651</v>
-      </c>
-      <c r="Q170">
-        <v>5.060599429861737</v>
-      </c>
-      <c r="R170">
-        <v>5.7422</v>
-      </c>
-      <c r="S170">
-        <v>5.633099999999999</v>
-      </c>
-      <c r="T170">
-        <v>8.9702</v>
-      </c>
-      <c r="U170">
-        <v>5.365799999999998</v>
-      </c>
-      <c r="V170">
-        <v>7.659800000000001</v>
-      </c>
-      <c r="W170">
-        <v>9.871000000000002</v>
-      </c>
-      <c r="X170">
-        <v>10.5376</v>
-      </c>
-      <c r="Y170">
-        <v>10.3989</v>
-      </c>
       <c r="Z170">
-        <v>8.907200000000001</v>
+        <v>0.3841</v>
       </c>
       <c r="AA170">
-        <v>8.200900000000001</v>
+        <v>-0.2419</v>
       </c>
       <c r="AB170">
-        <v>7.159900000000001</v>
+        <v>0.2551</v>
       </c>
       <c r="AC170">
-        <v>8.679700000000004</v>
+        <v>0.3417</v>
       </c>
       <c r="AD170">
-        <v>9.721264000000005</v>
+        <v>0</v>
       </c>
       <c r="AE170">
-        <v>10.40175248000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:31">
@@ -15188,7 +15227,7 @@
         <v>4</v>
       </c>
       <c r="B171" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C171" t="s">
         <v>193</v>
@@ -15196,86 +15235,35 @@
       <c r="D171" t="s">
         <v>194</v>
       </c>
-      <c r="E171">
-        <v>27.39165513</v>
-      </c>
-      <c r="F171">
-        <v>34.29965429999999</v>
-      </c>
-      <c r="G171">
-        <v>33.67331613</v>
-      </c>
-      <c r="H171">
-        <v>33.47762618</v>
-      </c>
-      <c r="I171">
-        <v>48.65726483</v>
-      </c>
-      <c r="J171">
-        <v>48.89512829</v>
-      </c>
-      <c r="K171">
-        <v>42.7878</v>
-      </c>
-      <c r="L171">
-        <v>55.9915</v>
-      </c>
-      <c r="M171">
-        <v>55.8556</v>
-      </c>
-      <c r="N171">
-        <v>56.8408</v>
-      </c>
-      <c r="O171">
-        <v>54.8424</v>
-      </c>
-      <c r="P171">
-        <v>62.3321</v>
-      </c>
-      <c r="Q171">
-        <v>71.443</v>
-      </c>
-      <c r="R171">
-        <v>79.90470000000001</v>
-      </c>
-      <c r="S171">
-        <v>88.3548</v>
-      </c>
-      <c r="T171">
-        <v>95.405</v>
-      </c>
-      <c r="U171">
-        <v>75.40100000000001</v>
-      </c>
       <c r="V171">
-        <v>91.1133</v>
+        <v>-1.252</v>
       </c>
       <c r="W171">
-        <v>108.4361</v>
+        <v>-1.013</v>
       </c>
       <c r="X171">
-        <v>110.8431</v>
+        <v>-2.2504</v>
       </c>
       <c r="Y171">
-        <v>114.1851</v>
+        <v>-2.0646</v>
       </c>
       <c r="Z171">
-        <v>119.6292</v>
+        <v>0.3841</v>
       </c>
       <c r="AA171">
-        <v>126.0022</v>
+        <v>-0.2419</v>
       </c>
       <c r="AB171">
-        <v>123.9707</v>
+        <v>0.2551</v>
       </c>
       <c r="AC171">
-        <v>128.6282</v>
+        <v>0.3417</v>
       </c>
       <c r="AD171">
-        <v>9.721264000000005</v>
+        <v>0</v>
       </c>
       <c r="AE171">
-        <v>10.40175248000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:31">
@@ -15283,7 +15271,7 @@
         <v>4</v>
       </c>
       <c r="B172" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C172" t="s">
         <v>193</v>
@@ -15292,19 +15280,19 @@
         <v>194</v>
       </c>
       <c r="Z172">
-        <v>0.3841</v>
+        <v>-0.0235</v>
       </c>
       <c r="AA172">
-        <v>-0.2419</v>
+        <v>0.0759</v>
       </c>
       <c r="AB172">
-        <v>0.2551</v>
+        <v>0.0939</v>
       </c>
       <c r="AC172">
-        <v>0.3417</v>
+        <v>0.0542</v>
       </c>
       <c r="AD172">
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="AE172">
         <v>0</v>
@@ -15315,7 +15303,7 @@
         <v>4</v>
       </c>
       <c r="B173" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C173" t="s">
         <v>193</v>
@@ -15324,31 +15312,31 @@
         <v>194</v>
       </c>
       <c r="V173">
-        <v>-1.252</v>
+        <v>2.434</v>
       </c>
       <c r="W173">
-        <v>-1.013</v>
+        <v>1.351</v>
       </c>
       <c r="X173">
-        <v>-2.2504</v>
+        <v>5.17705</v>
       </c>
       <c r="Y173">
-        <v>-2.0646</v>
+        <v>1.858</v>
       </c>
       <c r="Z173">
-        <v>0.3841</v>
+        <v>-0.0235</v>
       </c>
       <c r="AA173">
-        <v>-0.2419</v>
+        <v>0.0759</v>
       </c>
       <c r="AB173">
-        <v>0.2551</v>
+        <v>0.0939</v>
       </c>
       <c r="AC173">
-        <v>0.3417</v>
+        <v>0.0542</v>
       </c>
       <c r="AD173">
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="AE173">
         <v>0</v>
@@ -15359,7 +15347,7 @@
         <v>4</v>
       </c>
       <c r="B174" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C174" t="s">
         <v>193</v>
@@ -15367,35 +15355,23 @@
       <c r="D174" t="s">
         <v>194</v>
       </c>
-      <c r="V174">
-        <v>-1.252</v>
-      </c>
-      <c r="W174">
-        <v>-1.013</v>
-      </c>
-      <c r="X174">
-        <v>-2.2504</v>
-      </c>
-      <c r="Y174">
-        <v>-2.0646</v>
-      </c>
       <c r="Z174">
-        <v>-1.0655</v>
+        <v>-0.2212</v>
       </c>
       <c r="AA174">
-        <v>-3.153</v>
+        <v>0.08069999999999999</v>
       </c>
       <c r="AB174">
-        <v>-0.3143</v>
+        <v>-0.1096</v>
       </c>
       <c r="AC174">
-        <v>-2.5443</v>
+        <v>-0.017</v>
       </c>
       <c r="AD174">
-        <v>-0</v>
+        <v>-0.001</v>
       </c>
       <c r="AE174">
-        <v>0</v>
+        <v>-0.022</v>
       </c>
     </row>
     <row r="175" spans="1:31">
@@ -15403,7 +15379,7 @@
         <v>4</v>
       </c>
       <c r="B175" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C175" t="s">
         <v>193</v>
@@ -15411,23 +15387,35 @@
       <c r="D175" t="s">
         <v>194</v>
       </c>
+      <c r="V175">
+        <v>-0.145</v>
+      </c>
+      <c r="W175">
+        <v>0.503</v>
+      </c>
+      <c r="X175">
+        <v>1.567</v>
+      </c>
+      <c r="Y175">
+        <v>-3.3405</v>
+      </c>
       <c r="Z175">
-        <v>-0.0235</v>
+        <v>-0.2212</v>
       </c>
       <c r="AA175">
-        <v>0.0759</v>
+        <v>0.08069999999999999</v>
       </c>
       <c r="AB175">
-        <v>0.0939</v>
+        <v>-0.1096</v>
       </c>
       <c r="AC175">
-        <v>0.0542</v>
+        <v>-0.017</v>
       </c>
       <c r="AD175">
-        <v>0.1875</v>
+        <v>-0.001</v>
       </c>
       <c r="AE175">
-        <v>0</v>
+        <v>-0.022</v>
       </c>
     </row>
     <row r="176" spans="1:31">
@@ -15435,7 +15423,7 @@
         <v>4</v>
       </c>
       <c r="B176" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C176" t="s">
         <v>193</v>
@@ -15443,35 +15431,23 @@
       <c r="D176" t="s">
         <v>194</v>
       </c>
-      <c r="V176">
-        <v>2.434</v>
-      </c>
-      <c r="W176">
-        <v>1.351</v>
-      </c>
-      <c r="X176">
-        <v>5.17705</v>
-      </c>
-      <c r="Y176">
-        <v>1.858</v>
-      </c>
       <c r="Z176">
-        <v>-0.0235</v>
+        <v>0.3647</v>
       </c>
       <c r="AA176">
-        <v>0.0759</v>
+        <v>-0.2683</v>
       </c>
       <c r="AB176">
-        <v>0.0939</v>
+        <v>-0.1284</v>
       </c>
       <c r="AC176">
-        <v>0.0542</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="AD176">
-        <v>0.1875</v>
+        <v>-0.015</v>
       </c>
       <c r="AE176">
-        <v>0</v>
+        <v>-0.011</v>
       </c>
     </row>
     <row r="177" spans="1:31">
@@ -15479,7 +15455,7 @@
         <v>4</v>
       </c>
       <c r="B177" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C177" t="s">
         <v>193</v>
@@ -15488,34 +15464,34 @@
         <v>194</v>
       </c>
       <c r="V177">
-        <v>2.434</v>
+        <v>0</v>
       </c>
       <c r="W177">
-        <v>1.351</v>
+        <v>0</v>
       </c>
       <c r="X177">
-        <v>5.17705</v>
+        <v>0.6</v>
       </c>
       <c r="Y177">
-        <v>1.858</v>
+        <v>0.439</v>
       </c>
       <c r="Z177">
-        <v>-0.391</v>
+        <v>0.3647</v>
       </c>
       <c r="AA177">
-        <v>-0.7209899999999999</v>
+        <v>-0.2683</v>
       </c>
       <c r="AB177">
-        <v>-0.6191</v>
+        <v>-0.1284</v>
       </c>
       <c r="AC177">
-        <v>2.212</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="AD177">
-        <v>7.652214022140221</v>
+        <v>-0.015</v>
       </c>
       <c r="AE177">
-        <v>0</v>
+        <v>-0.011</v>
       </c>
     </row>
     <row r="178" spans="1:31">
@@ -15523,31 +15499,85 @@
         <v>4</v>
       </c>
       <c r="B178" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C178" t="s">
         <v>193</v>
       </c>
       <c r="D178" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="H178">
+        <v>92.64749999999999</v>
+      </c>
+      <c r="I178">
+        <v>100.4916666666667</v>
+      </c>
+      <c r="J178">
+        <v>105.7158333333333</v>
+      </c>
+      <c r="K178">
+        <v>107.93</v>
+      </c>
+      <c r="L178">
+        <v>105.97</v>
+      </c>
+      <c r="M178">
+        <v>103.1725</v>
+      </c>
+      <c r="N178">
+        <v>101.3783333333333</v>
+      </c>
+      <c r="O178">
+        <v>99.83166666666665</v>
+      </c>
+      <c r="P178">
+        <v>99.63083333333334</v>
+      </c>
+      <c r="Q178">
+        <v>98.98250000000002</v>
+      </c>
+      <c r="R178">
+        <v>98.85083333333334</v>
+      </c>
+      <c r="S178">
+        <v>98.63749999999999</v>
+      </c>
+      <c r="T178">
+        <v>100.4291666666667</v>
+      </c>
+      <c r="U178">
+        <v>100.6683333333333</v>
+      </c>
+      <c r="V178">
+        <v>97.77583333333334</v>
+      </c>
+      <c r="W178">
+        <v>97.13749999999999</v>
+      </c>
+      <c r="X178">
+        <v>98.22500000000001</v>
+      </c>
+      <c r="Y178">
+        <v>99.16416666666666</v>
       </c>
       <c r="Z178">
-        <v>-0.2212</v>
+        <v>99.23999999999999</v>
       </c>
       <c r="AA178">
-        <v>0.08069999999999999</v>
+        <v>100</v>
       </c>
       <c r="AB178">
-        <v>-0.1096</v>
+        <v>100.6866666666667</v>
       </c>
       <c r="AC178">
-        <v>-0.017</v>
+        <v>101.4108333333333</v>
       </c>
       <c r="AD178">
-        <v>-0.001</v>
+        <v>102.2023651777911</v>
       </c>
       <c r="AE178">
-        <v>-0.022</v>
+        <v>103.2542365085968</v>
       </c>
     </row>
     <row r="179" spans="1:31">
@@ -15555,43 +15585,85 @@
         <v>4</v>
       </c>
       <c r="B179" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C179" t="s">
         <v>193</v>
       </c>
       <c r="D179" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="H179">
+        <v>85.45999999999999</v>
+      </c>
+      <c r="I179">
+        <v>85.56333333000001</v>
+      </c>
+      <c r="J179">
+        <v>86.13916666999999</v>
+      </c>
+      <c r="K179">
+        <v>86.84416667000001</v>
+      </c>
+      <c r="L179">
+        <v>86.86750000000001</v>
+      </c>
+      <c r="M179">
+        <v>88.58916667</v>
+      </c>
+      <c r="N179">
+        <v>90.06</v>
+      </c>
+      <c r="O179">
+        <v>90.95333333000001</v>
+      </c>
+      <c r="P179">
+        <v>91.2325</v>
+      </c>
+      <c r="Q179">
+        <v>91.47750000000001</v>
+      </c>
+      <c r="R179">
+        <v>92.31583333</v>
+      </c>
+      <c r="S179">
+        <v>93.11666667</v>
+      </c>
+      <c r="T179">
+        <v>94.33</v>
+      </c>
+      <c r="U179">
+        <v>95.68916667000001</v>
       </c>
       <c r="V179">
-        <v>-0.145</v>
+        <v>96.45</v>
       </c>
       <c r="W179">
-        <v>0.503</v>
+        <v>97.37416666999999</v>
       </c>
       <c r="X179">
-        <v>1.567</v>
+        <v>98.24333333</v>
       </c>
       <c r="Y179">
-        <v>-3.3405</v>
+        <v>99.2075</v>
       </c>
       <c r="Z179">
-        <v>-0.2212</v>
+        <v>99.54000000000001</v>
       </c>
       <c r="AA179">
-        <v>0.08069999999999999</v>
+        <v>99.99916666999999</v>
       </c>
       <c r="AB179">
-        <v>-0.1096</v>
+        <v>101.0083333</v>
       </c>
       <c r="AC179">
-        <v>-0.017</v>
+        <v>101.8258333</v>
       </c>
       <c r="AD179">
-        <v>-0.001</v>
+        <v>102.6206043022308</v>
       </c>
       <c r="AE179">
-        <v>-0.022</v>
+        <v>103.6767801688823</v>
       </c>
     </row>
     <row r="180" spans="1:31">
@@ -15599,43 +15671,85 @@
         <v>4</v>
       </c>
       <c r="B180" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C180" t="s">
         <v>193</v>
       </c>
       <c r="D180" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="H180">
+        <v>31.1525</v>
+      </c>
+      <c r="I180">
+        <v>37.235</v>
+      </c>
+      <c r="J180">
+        <v>42.76</v>
+      </c>
+      <c r="K180">
+        <v>46.58333333333334</v>
+      </c>
+      <c r="L180">
+        <v>54.62666666666667</v>
+      </c>
+      <c r="M180">
+        <v>54.61083333333333</v>
+      </c>
+      <c r="N180">
+        <v>55.5325</v>
+      </c>
+      <c r="O180">
+        <v>56.13</v>
+      </c>
+      <c r="P180">
+        <v>57.6625</v>
+      </c>
+      <c r="Q180">
+        <v>61.83083333333334</v>
+      </c>
+      <c r="R180">
+        <v>66.52416666666666</v>
+      </c>
+      <c r="S180">
+        <v>71.0675</v>
+      </c>
+      <c r="T180">
+        <v>83.80499999999999</v>
+      </c>
+      <c r="U180">
+        <v>90.64833333333333</v>
       </c>
       <c r="V180">
-        <v>-0.145</v>
+        <v>100.0766666666667</v>
       </c>
       <c r="W180">
-        <v>0.503</v>
+        <v>112.1283333333333</v>
       </c>
       <c r="X180">
-        <v>1.567</v>
+        <v>119.5925</v>
       </c>
       <c r="Y180">
-        <v>-3.3405</v>
+        <v>118.1041666666667</v>
       </c>
       <c r="Z180">
-        <v>-0.545</v>
+        <v>113.4266666666667</v>
       </c>
       <c r="AA180">
-        <v>-0.647</v>
+        <v>99.99916666666667</v>
       </c>
       <c r="AB180">
-        <v>0.5660000000000001</v>
+        <v>92.815</v>
       </c>
       <c r="AC180">
-        <v>-0.627</v>
+        <v>97.16166666666668</v>
       </c>
       <c r="AD180">
-        <v>-0.03688235294117648</v>
+        <v>102.5625604400253</v>
       </c>
       <c r="AE180">
-        <v>-0.8114117647058825</v>
+        <v>103.7678881637022</v>
       </c>
     </row>
     <row r="181" spans="1:31">
@@ -15643,31 +15757,85 @@
         <v>4</v>
       </c>
       <c r="B181" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C181" t="s">
         <v>193</v>
       </c>
       <c r="D181" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="H181">
+        <v>57.81583333</v>
+      </c>
+      <c r="I181">
+        <v>59.64083333</v>
+      </c>
+      <c r="J181">
+        <v>57.51416667</v>
+      </c>
+      <c r="K181">
+        <v>58.6575</v>
+      </c>
+      <c r="L181">
+        <v>68.23083333</v>
+      </c>
+      <c r="M181">
+        <v>69.17</v>
+      </c>
+      <c r="N181">
+        <v>66.65666667000001</v>
+      </c>
+      <c r="O181">
+        <v>66.77416667</v>
+      </c>
+      <c r="P181">
+        <v>71.18000000000001</v>
+      </c>
+      <c r="Q181">
+        <v>80.22</v>
+      </c>
+      <c r="R181">
+        <v>86.05416667</v>
+      </c>
+      <c r="S181">
+        <v>86.24250000000001</v>
+      </c>
+      <c r="T181">
+        <v>103.3541667</v>
+      </c>
+      <c r="U181">
+        <v>88.90583332999999</v>
+      </c>
+      <c r="V181">
+        <v>97.77333333</v>
+      </c>
+      <c r="W181">
+        <v>114.4125</v>
+      </c>
+      <c r="X181">
+        <v>121.2708333</v>
+      </c>
+      <c r="Y181">
+        <v>115.6916667</v>
       </c>
       <c r="Z181">
-        <v>0.3647</v>
+        <v>108.6966667</v>
       </c>
       <c r="AA181">
-        <v>-0.2683</v>
+        <v>99.99916666999999</v>
       </c>
       <c r="AB181">
-        <v>-0.1284</v>
+        <v>99.40083333</v>
       </c>
       <c r="AC181">
-        <v>-0.008999999999999999</v>
+        <v>109.1933333</v>
       </c>
       <c r="AD181">
-        <v>-0.015</v>
+        <v>115.2630273897017</v>
       </c>
       <c r="AE181">
-        <v>-0.011</v>
+        <v>116.6176125505215</v>
       </c>
     </row>
     <row r="182" spans="1:31">
@@ -15675,43 +15843,85 @@
         <v>4</v>
       </c>
       <c r="B182" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C182" t="s">
         <v>193</v>
       </c>
       <c r="D182" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="H182">
+        <v>52.67416666666667</v>
+      </c>
+      <c r="I182">
+        <v>57.69333333333334</v>
+      </c>
+      <c r="J182">
+        <v>58.4025</v>
+      </c>
+      <c r="K182">
+        <v>58.04083333333333</v>
+      </c>
+      <c r="L182">
+        <v>55.8125</v>
+      </c>
+      <c r="M182">
+        <v>55.70166666666667</v>
+      </c>
+      <c r="N182">
+        <v>56.13500000000001</v>
+      </c>
+      <c r="O182">
+        <v>57.87916666666667</v>
+      </c>
+      <c r="P182">
+        <v>59.21083333333333</v>
+      </c>
+      <c r="Q182">
+        <v>60.04416666666666</v>
+      </c>
+      <c r="R182">
+        <v>61.68416666666666</v>
+      </c>
+      <c r="S182">
+        <v>68.12833333333333</v>
+      </c>
+      <c r="T182">
+        <v>78.96583333333334</v>
+      </c>
+      <c r="U182">
+        <v>83.56333333333333</v>
       </c>
       <c r="V182">
-        <v>0</v>
+        <v>87.92166666666667</v>
       </c>
       <c r="W182">
-        <v>0</v>
+        <v>94.09166666666665</v>
       </c>
       <c r="X182">
-        <v>0.6</v>
+        <v>97.045</v>
       </c>
       <c r="Y182">
-        <v>0.439</v>
+        <v>98.36</v>
       </c>
       <c r="Z182">
-        <v>0.3647</v>
+        <v>100.4741666666667</v>
       </c>
       <c r="AA182">
-        <v>-0.2683</v>
+        <v>100</v>
       </c>
       <c r="AB182">
-        <v>-0.1284</v>
+        <v>102.2291666666667</v>
       </c>
       <c r="AC182">
-        <v>-0.008999999999999999</v>
+        <v>109.5075</v>
       </c>
       <c r="AD182">
-        <v>-0.015</v>
+        <v>113.453857233265</v>
       </c>
       <c r="AE182">
-        <v>-0.011</v>
+        <v>116.9037994250425</v>
       </c>
     </row>
     <row r="183" spans="1:31">
@@ -15719,43 +15929,85 @@
         <v>4</v>
       </c>
       <c r="B183" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C183" t="s">
         <v>193</v>
       </c>
       <c r="D183" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="H183">
+        <v>63.28083333</v>
+      </c>
+      <c r="I183">
+        <v>64.705</v>
+      </c>
+      <c r="J183">
+        <v>65.61333333</v>
+      </c>
+      <c r="K183">
+        <v>66.02500000000001</v>
+      </c>
+      <c r="L183">
+        <v>66.88083333</v>
+      </c>
+      <c r="M183">
+        <v>68.33166667</v>
+      </c>
+      <c r="N183">
+        <v>69.34666667</v>
+      </c>
+      <c r="O183">
+        <v>71.255</v>
+      </c>
+      <c r="P183">
+        <v>72.83666667</v>
+      </c>
+      <c r="Q183">
+        <v>74.315</v>
+      </c>
+      <c r="R183">
+        <v>75.84</v>
+      </c>
+      <c r="S183">
+        <v>79.37416666999999</v>
+      </c>
+      <c r="T183">
+        <v>85.53749999999999</v>
+      </c>
+      <c r="U183">
+        <v>86.96333333</v>
       </c>
       <c r="V183">
-        <v>0</v>
+        <v>87.87083333</v>
       </c>
       <c r="W183">
-        <v>0</v>
+        <v>90.58916667</v>
       </c>
       <c r="X183">
-        <v>0.6</v>
+        <v>93.36666667</v>
       </c>
       <c r="Y183">
-        <v>0.439</v>
+        <v>96.36750000000001</v>
       </c>
       <c r="Z183">
-        <v>-0.08699999999999999</v>
+        <v>98.43166667</v>
       </c>
       <c r="AA183">
-        <v>-0.53</v>
+        <v>99.99916666999999</v>
       </c>
       <c r="AB183">
-        <v>0.183</v>
+        <v>103.4516667</v>
       </c>
       <c r="AC183">
-        <v>-0.08599999999999999</v>
+        <v>105.6691667</v>
       </c>
       <c r="AD183">
-        <v>-0.1433333333333333</v>
+        <v>109.4772006733774</v>
       </c>
       <c r="AE183">
-        <v>-0.1051111111111111</v>
+        <v>112.8062193850483</v>
       </c>
     </row>
     <row r="184" spans="1:31">
@@ -15763,7 +16015,7 @@
         <v>4</v>
       </c>
       <c r="B184" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C184" t="s">
         <v>193</v>
@@ -15772,76 +16024,76 @@
         <v>195</v>
       </c>
       <c r="H184">
-        <v>92.64749999999999</v>
+        <v>65.64333333333333</v>
       </c>
       <c r="I184">
-        <v>100.4916666666667</v>
+        <v>68.89666666666666</v>
       </c>
       <c r="J184">
-        <v>105.7158333333333</v>
+        <v>69.52583333333332</v>
       </c>
       <c r="K184">
-        <v>107.93</v>
+        <v>65.62166666666667</v>
       </c>
       <c r="L184">
-        <v>105.97</v>
+        <v>63.36833333333333</v>
       </c>
       <c r="M184">
-        <v>103.1725</v>
+        <v>69.05250000000001</v>
       </c>
       <c r="N184">
-        <v>101.3783333333333</v>
+        <v>67.54083333333334</v>
       </c>
       <c r="O184">
-        <v>99.83166666666665</v>
+        <v>59.44166666666667</v>
       </c>
       <c r="P184">
-        <v>99.63083333333334</v>
+        <v>60.92083333333333</v>
       </c>
       <c r="Q184">
-        <v>98.98250000000002</v>
+        <v>64.81166666666667</v>
       </c>
       <c r="R184">
-        <v>98.85083333333334</v>
+        <v>70.03749999999999</v>
       </c>
       <c r="S184">
-        <v>98.63749999999999</v>
+        <v>76.11666666666667</v>
       </c>
       <c r="T184">
-        <v>100.4291666666667</v>
+        <v>87.63416666666666</v>
       </c>
       <c r="U184">
-        <v>100.6683333333333</v>
+        <v>90.35666666666665</v>
       </c>
       <c r="V184">
-        <v>97.77583333333334</v>
+        <v>88.27083333333333</v>
       </c>
       <c r="W184">
-        <v>97.13749999999999</v>
+        <v>92.70833333333333</v>
       </c>
       <c r="X184">
-        <v>98.22500000000001</v>
+        <v>95.80833333333334</v>
       </c>
       <c r="Y184">
-        <v>99.16416666666666</v>
+        <v>98.91</v>
       </c>
       <c r="Z184">
-        <v>99.23999999999999</v>
+        <v>99.24333333333333</v>
       </c>
       <c r="AA184">
-        <v>100</v>
+        <v>100.0008333333333</v>
       </c>
       <c r="AB184">
-        <v>100.6866666666667</v>
+        <v>101.5158333333333</v>
       </c>
       <c r="AC184">
-        <v>101.4108333333333</v>
+        <v>103.1783333333333</v>
       </c>
       <c r="AD184">
-        <v>102.2023651777911</v>
+        <v>103.7242953583878</v>
       </c>
       <c r="AE184">
-        <v>103.2542365085968</v>
+        <v>104.6477563161146</v>
       </c>
     </row>
     <row r="185" spans="1:31">
@@ -15849,7 +16101,7 @@
         <v>4</v>
       </c>
       <c r="B185" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C185" t="s">
         <v>193</v>
@@ -15858,76 +16110,76 @@
         <v>195</v>
       </c>
       <c r="H185">
-        <v>85.45999999999999</v>
+        <v>66.68416667</v>
       </c>
       <c r="I185">
-        <v>85.56333333000001</v>
+        <v>68.47666667</v>
       </c>
       <c r="J185">
-        <v>86.13916666999999</v>
+        <v>69.9725</v>
       </c>
       <c r="K185">
-        <v>86.84416667000001</v>
+        <v>69.99083333</v>
       </c>
       <c r="L185">
-        <v>86.86750000000001</v>
+        <v>70.15666667000001</v>
       </c>
       <c r="M185">
-        <v>88.58916667</v>
+        <v>75.0175</v>
       </c>
       <c r="N185">
-        <v>90.06</v>
+        <v>77.425</v>
       </c>
       <c r="O185">
-        <v>90.95333333000001</v>
+        <v>78.75</v>
       </c>
       <c r="P185">
-        <v>91.2325</v>
+        <v>79.47083333</v>
       </c>
       <c r="Q185">
-        <v>91.47750000000001</v>
+        <v>80.81166666999999</v>
       </c>
       <c r="R185">
-        <v>92.31583333</v>
+        <v>83.43166667</v>
       </c>
       <c r="S185">
-        <v>93.11666667</v>
+        <v>85.94416667</v>
       </c>
       <c r="T185">
-        <v>94.33</v>
+        <v>88.32583332999999</v>
       </c>
       <c r="U185">
-        <v>95.68916667000001</v>
+        <v>88.64166667000001</v>
       </c>
       <c r="V185">
-        <v>96.45</v>
+        <v>91.7675</v>
       </c>
       <c r="W185">
-        <v>97.37416666999999</v>
+        <v>91.97583333</v>
       </c>
       <c r="X185">
-        <v>98.24333333</v>
+        <v>95.09916667</v>
       </c>
       <c r="Y185">
-        <v>99.2075</v>
+        <v>99.24666667</v>
       </c>
       <c r="Z185">
-        <v>99.54000000000001</v>
+        <v>97.9325</v>
       </c>
       <c r="AA185">
-        <v>99.99916666999999</v>
+        <v>100.0008333</v>
       </c>
       <c r="AB185">
-        <v>101.0083333</v>
+        <v>102.5633333</v>
       </c>
       <c r="AC185">
-        <v>101.8258333</v>
+        <v>102.6341667</v>
       </c>
       <c r="AD185">
-        <v>102.6206043022308</v>
+        <v>103.1772492996218</v>
       </c>
       <c r="AE185">
-        <v>103.6767801688823</v>
+        <v>104.0958398875321</v>
       </c>
     </row>
     <row r="186" spans="1:31">
@@ -15935,7 +16187,7 @@
         <v>4</v>
       </c>
       <c r="B186" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C186" t="s">
         <v>193</v>
@@ -15944,76 +16196,76 @@
         <v>195</v>
       </c>
       <c r="H186">
-        <v>31.1525</v>
+        <v>42.58</v>
       </c>
       <c r="I186">
-        <v>37.235</v>
+        <v>49.23916666666666</v>
       </c>
       <c r="J186">
-        <v>42.76</v>
+        <v>54.83750000000001</v>
       </c>
       <c r="K186">
-        <v>46.58333333333334</v>
+        <v>58.46083333333333</v>
       </c>
       <c r="L186">
-        <v>54.62666666666667</v>
+        <v>61.57083333333333</v>
       </c>
       <c r="M186">
-        <v>54.61083333333333</v>
+        <v>64.30916666666667</v>
       </c>
       <c r="N186">
-        <v>55.5325</v>
+        <v>66.39</v>
       </c>
       <c r="O186">
-        <v>56.13</v>
+        <v>66.59166666666667</v>
       </c>
       <c r="P186">
-        <v>57.6625</v>
+        <v>66.37916666666666</v>
       </c>
       <c r="Q186">
-        <v>61.83083333333334</v>
+        <v>68.58666666666667</v>
       </c>
       <c r="R186">
-        <v>66.52416666666666</v>
+        <v>71.9025</v>
       </c>
       <c r="S186">
-        <v>71.0675</v>
+        <v>76.79833333333333</v>
       </c>
       <c r="T186">
-        <v>83.80499999999999</v>
+        <v>86.1425</v>
       </c>
       <c r="U186">
-        <v>90.64833333333333</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="V186">
-        <v>100.0766666666667</v>
+        <v>89.73833333333334</v>
       </c>
       <c r="W186">
-        <v>112.1283333333333</v>
+        <v>90.86500000000001</v>
       </c>
       <c r="X186">
-        <v>119.5925</v>
+        <v>93.49166666666666</v>
       </c>
       <c r="Y186">
-        <v>118.1041666666667</v>
+        <v>95.22250000000001</v>
       </c>
       <c r="Z186">
-        <v>113.4266666666667</v>
+        <v>96.74833333333333</v>
       </c>
       <c r="AA186">
-        <v>99.99916666666667</v>
+        <v>100.0016666666667</v>
       </c>
       <c r="AB186">
-        <v>92.815</v>
+        <v>103.155</v>
       </c>
       <c r="AC186">
-        <v>97.16166666666668</v>
+        <v>108.3525</v>
       </c>
       <c r="AD186">
-        <v>102.5625604400253</v>
+        <v>112.7976710636909</v>
       </c>
       <c r="AE186">
-        <v>103.7678881637022</v>
+        <v>117.7330814675215</v>
       </c>
     </row>
     <row r="187" spans="1:31">
@@ -16021,7 +16273,7 @@
         <v>4</v>
       </c>
       <c r="B187" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C187" t="s">
         <v>193</v>
@@ -16030,76 +16282,76 @@
         <v>195</v>
       </c>
       <c r="H187">
-        <v>57.81583333</v>
+        <v>67.87333332999999</v>
       </c>
       <c r="I187">
-        <v>59.64083333</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="J187">
-        <v>57.51416667</v>
+        <v>70.14916667</v>
       </c>
       <c r="K187">
-        <v>58.6575</v>
+        <v>71.21666667</v>
       </c>
       <c r="L187">
-        <v>68.23083333</v>
+        <v>72.83083333</v>
       </c>
       <c r="M187">
-        <v>69.17</v>
+        <v>74.32333333</v>
       </c>
       <c r="N187">
-        <v>66.65666667000001</v>
+        <v>76.24833332999999</v>
       </c>
       <c r="O187">
-        <v>66.77416667</v>
+        <v>77.69166667</v>
       </c>
       <c r="P187">
-        <v>71.18000000000001</v>
+        <v>79.33750000000001</v>
       </c>
       <c r="Q187">
-        <v>80.22</v>
+        <v>81.01833333</v>
       </c>
       <c r="R187">
-        <v>86.05416667</v>
+        <v>82.69583333</v>
       </c>
       <c r="S187">
-        <v>86.24250000000001</v>
+        <v>84.27166667</v>
       </c>
       <c r="T187">
-        <v>103.3541667</v>
+        <v>86.17916667</v>
       </c>
       <c r="U187">
-        <v>88.90583332999999</v>
+        <v>88.45</v>
       </c>
       <c r="V187">
-        <v>97.77333333</v>
+        <v>89.68583332999999</v>
       </c>
       <c r="W187">
-        <v>114.4125</v>
+        <v>91.41083333</v>
       </c>
       <c r="X187">
-        <v>121.2708333</v>
+        <v>93.73083333</v>
       </c>
       <c r="Y187">
-        <v>115.6916667</v>
+        <v>95.49333333</v>
       </c>
       <c r="Z187">
-        <v>108.6966667</v>
+        <v>97.64166667000001</v>
       </c>
       <c r="AA187">
-        <v>99.99916666999999</v>
+        <v>100</v>
       </c>
       <c r="AB187">
-        <v>99.40083333</v>
+        <v>102.2316667</v>
       </c>
       <c r="AC187">
-        <v>109.1933333</v>
+        <v>104.1816667</v>
       </c>
       <c r="AD187">
-        <v>115.2630273897017</v>
+        <v>108.455728952204</v>
       </c>
       <c r="AE187">
-        <v>116.6176125505215</v>
+        <v>113.2011596687965</v>
       </c>
     </row>
     <row r="188" spans="1:31">
@@ -16107,7 +16359,7 @@
         <v>4</v>
       </c>
       <c r="B188" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C188" t="s">
         <v>193</v>
@@ -16116,76 +16368,76 @@
         <v>195</v>
       </c>
       <c r="H188">
-        <v>52.67416666666667</v>
+        <v>62.90583333333333</v>
       </c>
       <c r="I188">
-        <v>57.69333333333334</v>
+        <v>69.40833333333333</v>
       </c>
       <c r="J188">
-        <v>58.4025</v>
+        <v>72.52</v>
       </c>
       <c r="K188">
-        <v>58.04083333333333</v>
+        <v>73.77</v>
       </c>
       <c r="L188">
-        <v>55.8125</v>
+        <v>72.94333333333333</v>
       </c>
       <c r="M188">
-        <v>55.70166666666667</v>
+        <v>72.9875</v>
       </c>
       <c r="N188">
-        <v>56.13500000000001</v>
+        <v>73.41833333333334</v>
       </c>
       <c r="O188">
-        <v>57.87916666666667</v>
+        <v>73.92333333333333</v>
       </c>
       <c r="P188">
-        <v>59.21083333333333</v>
+        <v>74.39750000000001</v>
       </c>
       <c r="Q188">
-        <v>60.04416666666666</v>
+        <v>75.34583333333333</v>
       </c>
       <c r="R188">
-        <v>61.68416666666666</v>
+        <v>77.145</v>
       </c>
       <c r="S188">
-        <v>68.12833333333333</v>
+        <v>81.16666666666667</v>
       </c>
       <c r="T188">
-        <v>78.96583333333334</v>
+        <v>88.71847965410413</v>
       </c>
       <c r="U188">
-        <v>83.56333333333333</v>
+        <v>91.97128959677305</v>
       </c>
       <c r="V188">
-        <v>87.92166666666667</v>
+        <v>91.94094260426945</v>
       </c>
       <c r="W188">
-        <v>94.09166666666665</v>
+        <v>94.13397481977555</v>
       </c>
       <c r="X188">
-        <v>97.045</v>
+        <v>96.37345961048149</v>
       </c>
       <c r="Y188">
-        <v>98.36</v>
+        <v>97.72130451674201</v>
       </c>
       <c r="Z188">
-        <v>100.4741666666667</v>
+        <v>98.79762654833354</v>
       </c>
       <c r="AA188">
-        <v>100</v>
+        <v>100.0169095670175</v>
       </c>
       <c r="AB188">
-        <v>102.2291666666667</v>
+        <v>101.876892929928</v>
       </c>
       <c r="AC188">
-        <v>109.5075</v>
+        <v>105.7829055373266</v>
       </c>
       <c r="AD188">
-        <v>113.453857233265</v>
+        <v>108.5630722850966</v>
       </c>
       <c r="AE188">
-        <v>116.9037994250425</v>
+        <v>111.4598683070769</v>
       </c>
     </row>
     <row r="189" spans="1:31">
@@ -16193,7 +16445,7 @@
         <v>4</v>
       </c>
       <c r="B189" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C189" t="s">
         <v>193</v>
@@ -16202,591 +16454,75 @@
         <v>195</v>
       </c>
       <c r="H189">
-        <v>63.28083333</v>
+        <v>73.31666667</v>
       </c>
       <c r="I189">
-        <v>64.705</v>
+        <v>74.13833332999999</v>
       </c>
       <c r="J189">
-        <v>65.61333333</v>
+        <v>75.01916667</v>
       </c>
       <c r="K189">
-        <v>66.02500000000001</v>
+        <v>75.8075</v>
       </c>
       <c r="L189">
-        <v>66.88083333</v>
+        <v>76.67</v>
       </c>
       <c r="M189">
-        <v>68.33166667</v>
+        <v>78.26000000000001</v>
       </c>
       <c r="N189">
-        <v>69.34666667</v>
+        <v>79.8725</v>
       </c>
       <c r="O189">
-        <v>71.255</v>
+        <v>81.2</v>
       </c>
       <c r="P189">
-        <v>72.83666667</v>
+        <v>82.3475</v>
       </c>
       <c r="Q189">
-        <v>74.315</v>
+        <v>83.48083333</v>
       </c>
       <c r="R189">
-        <v>75.84</v>
+        <v>84.8275</v>
       </c>
       <c r="S189">
-        <v>79.37416666999999</v>
+        <v>86.44083333</v>
       </c>
       <c r="T189">
-        <v>85.53749999999999</v>
+        <v>88.78749999999999</v>
       </c>
       <c r="U189">
-        <v>86.96333333</v>
+        <v>90.58666667</v>
       </c>
       <c r="V189">
-        <v>87.87083333</v>
+        <v>91.61666667</v>
       </c>
       <c r="W189">
-        <v>90.58916667</v>
+        <v>93.25749999999999</v>
       </c>
       <c r="X189">
-        <v>93.36666667</v>
+        <v>95.18000000000001</v>
       </c>
       <c r="Y189">
-        <v>96.36750000000001</v>
+        <v>96.88083333</v>
       </c>
       <c r="Z189">
-        <v>98.43166667</v>
+        <v>98.405</v>
       </c>
       <c r="AA189">
-        <v>99.99916666999999</v>
+        <v>100.0008333</v>
       </c>
       <c r="AB189">
-        <v>103.4516667</v>
+        <v>102.0191667</v>
       </c>
       <c r="AC189">
-        <v>105.6691667</v>
+        <v>103.6441667</v>
       </c>
       <c r="AD189">
-        <v>109.4772006733774</v>
+        <v>106.3681235094298</v>
       </c>
       <c r="AE189">
-        <v>112.8062193850483</v>
-      </c>
-    </row>
-    <row r="190" spans="1:31">
-      <c r="A190" t="s">
-        <v>4</v>
-      </c>
-      <c r="B190" t="s">
-        <v>187</v>
-      </c>
-      <c r="C190" t="s">
-        <v>193</v>
-      </c>
-      <c r="D190" t="s">
-        <v>195</v>
-      </c>
-      <c r="H190">
-        <v>65.64333333333333</v>
-      </c>
-      <c r="I190">
-        <v>68.89666666666666</v>
-      </c>
-      <c r="J190">
-        <v>69.52583333333332</v>
-      </c>
-      <c r="K190">
-        <v>65.62166666666667</v>
-      </c>
-      <c r="L190">
-        <v>63.36833333333333</v>
-      </c>
-      <c r="M190">
-        <v>69.05250000000001</v>
-      </c>
-      <c r="N190">
-        <v>67.54083333333334</v>
-      </c>
-      <c r="O190">
-        <v>59.44166666666667</v>
-      </c>
-      <c r="P190">
-        <v>60.92083333333333</v>
-      </c>
-      <c r="Q190">
-        <v>64.81166666666667</v>
-      </c>
-      <c r="R190">
-        <v>70.03749999999999</v>
-      </c>
-      <c r="S190">
-        <v>76.11666666666667</v>
-      </c>
-      <c r="T190">
-        <v>87.63416666666666</v>
-      </c>
-      <c r="U190">
-        <v>90.35666666666665</v>
-      </c>
-      <c r="V190">
-        <v>88.27083333333333</v>
-      </c>
-      <c r="W190">
-        <v>92.70833333333333</v>
-      </c>
-      <c r="X190">
-        <v>95.80833333333334</v>
-      </c>
-      <c r="Y190">
-        <v>98.91</v>
-      </c>
-      <c r="Z190">
-        <v>99.24333333333333</v>
-      </c>
-      <c r="AA190">
-        <v>100.0008333333333</v>
-      </c>
-      <c r="AB190">
-        <v>101.5158333333333</v>
-      </c>
-      <c r="AC190">
-        <v>103.1783333333333</v>
-      </c>
-      <c r="AD190">
-        <v>103.7242953583878</v>
-      </c>
-      <c r="AE190">
-        <v>104.6477563161146</v>
-      </c>
-    </row>
-    <row r="191" spans="1:31">
-      <c r="A191" t="s">
-        <v>4</v>
-      </c>
-      <c r="B191" t="s">
-        <v>188</v>
-      </c>
-      <c r="C191" t="s">
-        <v>193</v>
-      </c>
-      <c r="D191" t="s">
-        <v>195</v>
-      </c>
-      <c r="H191">
-        <v>66.68416667</v>
-      </c>
-      <c r="I191">
-        <v>68.47666667</v>
-      </c>
-      <c r="J191">
-        <v>69.9725</v>
-      </c>
-      <c r="K191">
-        <v>69.99083333</v>
-      </c>
-      <c r="L191">
-        <v>70.15666667000001</v>
-      </c>
-      <c r="M191">
-        <v>75.0175</v>
-      </c>
-      <c r="N191">
-        <v>77.425</v>
-      </c>
-      <c r="O191">
-        <v>78.75</v>
-      </c>
-      <c r="P191">
-        <v>79.47083333</v>
-      </c>
-      <c r="Q191">
-        <v>80.81166666999999</v>
-      </c>
-      <c r="R191">
-        <v>83.43166667</v>
-      </c>
-      <c r="S191">
-        <v>85.94416667</v>
-      </c>
-      <c r="T191">
-        <v>88.32583332999999</v>
-      </c>
-      <c r="U191">
-        <v>88.64166667000001</v>
-      </c>
-      <c r="V191">
-        <v>91.7675</v>
-      </c>
-      <c r="W191">
-        <v>91.97583333</v>
-      </c>
-      <c r="X191">
-        <v>95.09916667</v>
-      </c>
-      <c r="Y191">
-        <v>99.24666667</v>
-      </c>
-      <c r="Z191">
-        <v>97.9325</v>
-      </c>
-      <c r="AA191">
-        <v>100.0008333</v>
-      </c>
-      <c r="AB191">
-        <v>102.5633333</v>
-      </c>
-      <c r="AC191">
-        <v>102.6341667</v>
-      </c>
-      <c r="AD191">
-        <v>103.1772492996218</v>
-      </c>
-      <c r="AE191">
-        <v>104.0958398875321</v>
-      </c>
-    </row>
-    <row r="192" spans="1:31">
-      <c r="A192" t="s">
-        <v>4</v>
-      </c>
-      <c r="B192" t="s">
-        <v>189</v>
-      </c>
-      <c r="C192" t="s">
-        <v>193</v>
-      </c>
-      <c r="D192" t="s">
-        <v>195</v>
-      </c>
-      <c r="H192">
-        <v>42.58</v>
-      </c>
-      <c r="I192">
-        <v>49.23916666666666</v>
-      </c>
-      <c r="J192">
-        <v>54.83750000000001</v>
-      </c>
-      <c r="K192">
-        <v>58.46083333333333</v>
-      </c>
-      <c r="L192">
-        <v>61.57083333333333</v>
-      </c>
-      <c r="M192">
-        <v>64.30916666666667</v>
-      </c>
-      <c r="N192">
-        <v>66.39</v>
-      </c>
-      <c r="O192">
-        <v>66.59166666666667</v>
-      </c>
-      <c r="P192">
-        <v>66.37916666666666</v>
-      </c>
-      <c r="Q192">
-        <v>68.58666666666667</v>
-      </c>
-      <c r="R192">
-        <v>71.9025</v>
-      </c>
-      <c r="S192">
-        <v>76.79833333333333</v>
-      </c>
-      <c r="T192">
-        <v>86.1425</v>
-      </c>
-      <c r="U192">
-        <v>91.09999999999999</v>
-      </c>
-      <c r="V192">
-        <v>89.73833333333334</v>
-      </c>
-      <c r="W192">
-        <v>90.86500000000001</v>
-      </c>
-      <c r="X192">
-        <v>93.49166666666666</v>
-      </c>
-      <c r="Y192">
-        <v>95.22250000000001</v>
-      </c>
-      <c r="Z192">
-        <v>96.74833333333333</v>
-      </c>
-      <c r="AA192">
-        <v>100.0016666666667</v>
-      </c>
-      <c r="AB192">
-        <v>103.155</v>
-      </c>
-      <c r="AC192">
-        <v>108.3525</v>
-      </c>
-      <c r="AD192">
-        <v>112.7976710636909</v>
-      </c>
-      <c r="AE192">
-        <v>117.7330814675215</v>
-      </c>
-    </row>
-    <row r="193" spans="1:31">
-      <c r="A193" t="s">
-        <v>4</v>
-      </c>
-      <c r="B193" t="s">
-        <v>190</v>
-      </c>
-      <c r="C193" t="s">
-        <v>193</v>
-      </c>
-      <c r="D193" t="s">
-        <v>195</v>
-      </c>
-      <c r="H193">
-        <v>67.87333332999999</v>
-      </c>
-      <c r="I193">
-        <v>69.01000000000001</v>
-      </c>
-      <c r="J193">
-        <v>70.14916667</v>
-      </c>
-      <c r="K193">
-        <v>71.21666667</v>
-      </c>
-      <c r="L193">
-        <v>72.83083333</v>
-      </c>
-      <c r="M193">
-        <v>74.32333333</v>
-      </c>
-      <c r="N193">
-        <v>76.24833332999999</v>
-      </c>
-      <c r="O193">
-        <v>77.69166667</v>
-      </c>
-      <c r="P193">
-        <v>79.33750000000001</v>
-      </c>
-      <c r="Q193">
-        <v>81.01833333</v>
-      </c>
-      <c r="R193">
-        <v>82.69583333</v>
-      </c>
-      <c r="S193">
-        <v>84.27166667</v>
-      </c>
-      <c r="T193">
-        <v>86.17916667</v>
-      </c>
-      <c r="U193">
-        <v>88.45</v>
-      </c>
-      <c r="V193">
-        <v>89.68583332999999</v>
-      </c>
-      <c r="W193">
-        <v>91.41083333</v>
-      </c>
-      <c r="X193">
-        <v>93.73083333</v>
-      </c>
-      <c r="Y193">
-        <v>95.49333333</v>
-      </c>
-      <c r="Z193">
-        <v>97.64166667000001</v>
-      </c>
-      <c r="AA193">
-        <v>100</v>
-      </c>
-      <c r="AB193">
-        <v>102.2316667</v>
-      </c>
-      <c r="AC193">
-        <v>104.1816667</v>
-      </c>
-      <c r="AD193">
-        <v>108.455728952204</v>
-      </c>
-      <c r="AE193">
-        <v>113.2011596687965</v>
-      </c>
-    </row>
-    <row r="194" spans="1:31">
-      <c r="A194" t="s">
-        <v>4</v>
-      </c>
-      <c r="B194" t="s">
-        <v>191</v>
-      </c>
-      <c r="C194" t="s">
-        <v>193</v>
-      </c>
-      <c r="D194" t="s">
-        <v>195</v>
-      </c>
-      <c r="H194">
-        <v>62.90583333333333</v>
-      </c>
-      <c r="I194">
-        <v>69.40833333333333</v>
-      </c>
-      <c r="J194">
-        <v>72.52</v>
-      </c>
-      <c r="K194">
-        <v>73.77</v>
-      </c>
-      <c r="L194">
-        <v>72.94333333333333</v>
-      </c>
-      <c r="M194">
-        <v>72.9875</v>
-      </c>
-      <c r="N194">
-        <v>73.41833333333334</v>
-      </c>
-      <c r="O194">
-        <v>73.92333333333333</v>
-      </c>
-      <c r="P194">
-        <v>74.39750000000001</v>
-      </c>
-      <c r="Q194">
-        <v>75.34583333333333</v>
-      </c>
-      <c r="R194">
-        <v>77.145</v>
-      </c>
-      <c r="S194">
-        <v>81.16666666666667</v>
-      </c>
-      <c r="T194">
-        <v>88.71847965410413</v>
-      </c>
-      <c r="U194">
-        <v>91.97128959677305</v>
-      </c>
-      <c r="V194">
-        <v>91.94094260426945</v>
-      </c>
-      <c r="W194">
-        <v>94.13397481977555</v>
-      </c>
-      <c r="X194">
-        <v>96.37345961048149</v>
-      </c>
-      <c r="Y194">
-        <v>97.72130451674201</v>
-      </c>
-      <c r="Z194">
-        <v>98.79762654833354</v>
-      </c>
-      <c r="AA194">
-        <v>100.0169095670175</v>
-      </c>
-      <c r="AB194">
-        <v>101.876892929928</v>
-      </c>
-      <c r="AC194">
-        <v>105.7829055373266</v>
-      </c>
-      <c r="AD194">
-        <v>108.5630722850966</v>
-      </c>
-      <c r="AE194">
-        <v>111.4598683070769</v>
-      </c>
-    </row>
-    <row r="195" spans="1:31">
-      <c r="A195" t="s">
-        <v>4</v>
-      </c>
-      <c r="B195" t="s">
-        <v>192</v>
-      </c>
-      <c r="C195" t="s">
-        <v>193</v>
-      </c>
-      <c r="D195" t="s">
-        <v>195</v>
-      </c>
-      <c r="H195">
-        <v>73.31666667</v>
-      </c>
-      <c r="I195">
-        <v>74.13833332999999</v>
-      </c>
-      <c r="J195">
-        <v>75.01916667</v>
-      </c>
-      <c r="K195">
-        <v>75.8075</v>
-      </c>
-      <c r="L195">
-        <v>76.67</v>
-      </c>
-      <c r="M195">
-        <v>78.26000000000001</v>
-      </c>
-      <c r="N195">
-        <v>79.8725</v>
-      </c>
-      <c r="O195">
-        <v>81.2</v>
-      </c>
-      <c r="P195">
-        <v>82.3475</v>
-      </c>
-      <c r="Q195">
-        <v>83.48083333</v>
-      </c>
-      <c r="R195">
-        <v>84.8275</v>
-      </c>
-      <c r="S195">
-        <v>86.44083333</v>
-      </c>
-      <c r="T195">
-        <v>88.78749999999999</v>
-      </c>
-      <c r="U195">
-        <v>90.58666667</v>
-      </c>
-      <c r="V195">
-        <v>91.61666667</v>
-      </c>
-      <c r="W195">
-        <v>93.25749999999999</v>
-      </c>
-      <c r="X195">
-        <v>95.18000000000001</v>
-      </c>
-      <c r="Y195">
-        <v>96.88083333</v>
-      </c>
-      <c r="Z195">
-        <v>98.405</v>
-      </c>
-      <c r="AA195">
-        <v>100.0008333</v>
-      </c>
-      <c r="AB195">
-        <v>102.0191667</v>
-      </c>
-      <c r="AC195">
-        <v>103.6441667</v>
-      </c>
-      <c r="AD195">
-        <v>106.3681235094298</v>
-      </c>
-      <c r="AE195">
         <v>109.2063515602946</v>
       </c>
     </row>

</xml_diff>